<commit_message>
Updated database design. Added extra column to store wmts map data preferred format. Related to Issue [WTI-1087]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@8008 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 0c4540e02044ce8822be7eade2f73997cc49cb6a
Former-commit-id: 395051a1b6d34b065719060ef70fc9dfd04376c3
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" tabRatio="1000" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" tabRatio="1000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="470">
   <si>
     <t>Description</t>
   </si>
@@ -1534,6 +1534,9 @@
   </si>
   <si>
     <t>FlowVelocityStructureClosable.CoefficientOfVariation</t>
+  </si>
+  <si>
+    <t>PreferredFormat</t>
   </si>
 </sst>
 </file>
@@ -4087,10 +4090,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C110"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C107" sqref="C107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4643,41 +4646,44 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
+      <c r="A105" s="46" t="s">
         <v>460</v>
       </c>
-      <c r="B105" s="6" t="s">
+      <c r="B105" s="46" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
-        <v>467</v>
-      </c>
-      <c r="B106" s="6" t="s">
+      <c r="A106" s="8"/>
+      <c r="B106" s="46" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="6" t="s">
+      <c r="B107" s="46" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="6" t="s">
+      <c r="B108" s="46" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="6" t="s">
+      <c r="B109" s="46" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B110" s="46" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="5" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="5" t="s">
         <v>465</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C111" t="s">
         <v>466</v>
       </c>
     </row>
@@ -4718,10 +4724,9 @@
     <hyperlink ref="B47" location="HydraulicBoundaryLocationOutput" display="WaveHeightOutput"/>
     <hyperlink ref="B30" location="WmtsMapData" display="BackgroundMapData"/>
     <hyperlink ref="C30" r:id="rId2"/>
-    <hyperlink ref="A106" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId4"/>
+  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -6378,7 +6383,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated opslagmapping. Related to Issue [WTI-1087]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@8028 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 9f367e4c5cfab15ea79739deca4e2994bbf1de3e
Former-commit-id: 467d837cd6a225a53d0e4191b79ccc78b88ac73f
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="469">
   <si>
     <t>Description</t>
   </si>
@@ -1507,9 +1507,6 @@
   </si>
   <si>
     <t>BackgroundMapData</t>
-  </si>
-  <si>
-    <t>WmtsMapData</t>
   </si>
   <si>
     <t>IsVisible</t>
@@ -3361,7 +3358,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C57" s="44" t="s">
         <v>118</v>
@@ -3770,7 +3767,7 @@
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C138" s="44" t="s">
         <v>118</v>
@@ -4092,8 +4089,8 @@
   </sheetPr>
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C107" sqref="C107"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4260,7 +4257,7 @@
         <v>459</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -4647,7 +4644,7 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="46" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B105" s="46" t="s">
         <v>1</v>
@@ -4656,35 +4653,35 @@
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="8"/>
       <c r="B106" s="46" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B107" s="46" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" s="46" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B109" s="46" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B110" s="46" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
+        <v>464</v>
+      </c>
+      <c r="C111" t="s">
         <v>465</v>
-      </c>
-      <c r="C111" t="s">
-        <v>466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated database to include the storage of the sourcepath of the SurfaceLines in the PipingFailureMechanismMetaEntity
Related to Issue [WTI-1083]


git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@8074 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: d32a48e1230e3ad95e84a66e5a2a8dfda63b7aaf
Former-commit-id: 93a4a48303581fd777593994785ae1d67358e652
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" tabRatio="1000" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" tabRatio="1000" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="WaveImpactAsphalt" sheetId="10" r:id="rId20"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Piping!$B$154:$D$154</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Piping!$B$156:$D$156</definedName>
     <definedName name="AssessmentSection">General!$A$5</definedName>
     <definedName name="BreakWater">General!$A$77</definedName>
     <definedName name="CalculationGroup">General!$A$59</definedName>
@@ -52,7 +52,7 @@
     <definedName name="GeneralGrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$14</definedName>
     <definedName name="GeneralGrassCoverErosionOutwardsInput">GrassCoverErosionOutwards!$A$29</definedName>
     <definedName name="GeneralHeightStructuresInput">HeightStructures!$A$33</definedName>
-    <definedName name="GeneralPipingInput">Piping!$A$59</definedName>
+    <definedName name="GeneralPipingInput">Piping!$A$61</definedName>
     <definedName name="GeneralStabilityCoverWaveConditionsInput">StabilityStoneCover!$A$14</definedName>
     <definedName name="GeneralStabilityPointStructuresInput">StabilityPointStructures!$A$21</definedName>
     <definedName name="GeneralWaveImpactAsphaltCoverWaveConditionsInput">WaveImpactAsphalt!$A$28</definedName>
@@ -84,15 +84,15 @@
     <definedName name="MacrostabilityOutwardsFailureMechanismSectionResult">MacrostabilityOutwards!$A$11</definedName>
     <definedName name="MicrostabilityFailureMechanism">Microstability!$A$1</definedName>
     <definedName name="MicrostabilityFailureMechanismSectionResult">Microstability!$A$11</definedName>
-    <definedName name="PipingCalculationScenario">Piping!$A$75</definedName>
+    <definedName name="PipingCalculationScenario">Piping!$A$77</definedName>
     <definedName name="PipingFailureMechanism">Piping!$A$1</definedName>
-    <definedName name="PipingFailureMechanismSectionResult">Piping!$A$151</definedName>
-    <definedName name="PipingInput">Piping!$A$86</definedName>
-    <definedName name="PipingOutput">Piping!$A$124</definedName>
-    <definedName name="PipingProbabilityAssessmentInput">Piping!$A$71</definedName>
-    <definedName name="PipingSemiProbabilisticOutput">Piping!$A$136</definedName>
-    <definedName name="PipingSoilLayer">Piping!$A$47</definedName>
-    <definedName name="PipingSoilProfile">Piping!$A$41</definedName>
+    <definedName name="PipingFailureMechanismSectionResult">Piping!$A$153</definedName>
+    <definedName name="PipingInput">Piping!$A$88</definedName>
+    <definedName name="PipingOutput">Piping!$A$126</definedName>
+    <definedName name="PipingProbabilityAssessmentInput">Piping!$A$73</definedName>
+    <definedName name="PipingSemiProbabilisticOutput">Piping!$A$138</definedName>
+    <definedName name="PipingSoilLayer">Piping!$A$49</definedName>
+    <definedName name="PipingSoilProfile">Piping!$A$43</definedName>
     <definedName name="PipingStructureFailureMechanism">PipingStructure!$A$1</definedName>
     <definedName name="PipingStructureFailureMechanismSectionResult">PipingStructure!$A$11</definedName>
     <definedName name="ProbabilityAssessmentOutput">General!$A$63</definedName>
@@ -105,8 +105,8 @@
     <definedName name="StabilityStoneCoverFailureMechanism">StabilityStoneCover!$A$1</definedName>
     <definedName name="StabilityStoneCoverFailureMechanismSectionResult">StabilityStoneCover!$A$31</definedName>
     <definedName name="StabilityStoneCoverWaveConditionsOutput">StabilityStoneCover!$A$27</definedName>
-    <definedName name="StochasticSoilModel">Piping!$A$30</definedName>
-    <definedName name="StochasticSoilProfile">Piping!$A$36</definedName>
+    <definedName name="StochasticSoilModel">Piping!$A$32</definedName>
+    <definedName name="StochasticSoilProfile">Piping!$A$38</definedName>
     <definedName name="StrengthStabilityLengthwiseConstructionFailureMechanism">StrengthStabilityLengthwise!$A$1</definedName>
     <definedName name="StrengthStabilityLengthwiseConstructionFailureMechanismSectionResult">StrengthStabilityLengthwise!$A$11</definedName>
     <definedName name="StrengthStabilityPointConstructionFailureMechanism">StabilityPointStructures!$A$1</definedName>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="470">
   <si>
     <t>Description</t>
   </si>
@@ -1534,6 +1534,9 @@
   </si>
   <si>
     <t>PreferredFormat</t>
+  </si>
+  <si>
+    <t>SurfaceLineCollection</t>
   </si>
 </sst>
 </file>
@@ -4089,7 +4092,7 @@
   </sheetPr>
   <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
@@ -4939,10 +4942,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5119,203 +5122,196 @@
         <v>458</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="B30" s="46" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B32" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C32" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="31" spans="1:3" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="3" t="s">
+    <row r="33" spans="1:3" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B32" s="3" t="s">
+    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B33" s="3" t="s">
+    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B35" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B34" s="9" t="s">
+    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A36" s="7" t="s">
+    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B37" s="5" t="s">
+    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B39" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B38" s="3" t="s">
+    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B39" s="9" t="s">
+    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B41" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B43" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B42" s="3" t="s">
+    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B43" s="3" t="s">
+    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B44" s="9" t="s">
+    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B46" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B49" s="3" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="3" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>264</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B54" s="3" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B53" s="3" t="s">
+    <row r="55" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B55" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B54" s="3" t="s">
+    <row r="56" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B56" s="3" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B55" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B56" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="46" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B61" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="D59" s="44"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B60" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="C60" s="44" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C61" s="44" t="s">
-        <v>118</v>
-      </c>
+      <c r="D61" s="44"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="C62" t="s">
+        <v>139</v>
+      </c>
+      <c r="C62" s="44" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" s="44" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C64" t="s">
         <v>118</v>
@@ -5323,7 +5319,7 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C65" t="s">
         <v>118</v>
@@ -5331,7 +5327,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C66" t="s">
         <v>118</v>
@@ -5339,7 +5335,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C67" t="s">
         <v>118</v>
@@ -5347,7 +5343,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C68" t="s">
         <v>118</v>
@@ -5355,168 +5351,168 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="C69" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C69" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
+      <c r="C71" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B73" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="5" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="C72" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="5" t="s">
+      <c r="C74" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C75" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B77" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="9" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="9" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="9" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C79" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="3" t="s">
-        <v>26</v>
+      <c r="B81" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="5" t="s">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C85" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="5" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C86" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="B86" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="3" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>127</v>
+        <v>34</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B92" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="46" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="46" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="46" t="s">
+    <row r="95" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="46" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="C94" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C95" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B96" s="5" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="C96" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="C97" t="s">
         <v>168</v>
@@ -5524,7 +5520,7 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C98" t="s">
         <v>168</v>
@@ -5532,7 +5528,7 @@
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="C99" t="s">
         <v>168</v>
@@ -5540,7 +5536,7 @@
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C100" t="s">
         <v>168</v>
@@ -5548,7 +5544,7 @@
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C101" t="s">
         <v>168</v>
@@ -5556,7 +5552,7 @@
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C102" t="s">
         <v>168</v>
@@ -5564,7 +5560,7 @@
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="C103" t="s">
         <v>168</v>
@@ -5572,7 +5568,7 @@
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C104" t="s">
         <v>168</v>
@@ -5580,57 +5576,57 @@
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C105" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C106" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B107" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C107" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="3" t="s">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B109" s="3" t="s">
         <v>171</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="C108" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C109" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C110" t="s">
-        <v>276</v>
+        <v>167</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="C111" t="s">
-        <v>276</v>
+        <v>167</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C112" t="s">
         <v>276</v>
@@ -5638,7 +5634,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C113" t="s">
         <v>276</v>
@@ -5646,23 +5642,23 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114" s="5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C114" t="s">
-        <v>167</v>
+        <v>276</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C115" t="s">
-        <v>167</v>
+        <v>276</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C116" t="s">
         <v>167</v>
@@ -5670,208 +5666,224 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C117" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B118" s="3" t="s">
+      <c r="B118" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C118" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C119" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B119" s="3" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="3" t="s">
         <v>177</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B120" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C120" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B121" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C121" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122" s="5" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="C122" t="s">
         <v>276</v>
       </c>
     </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B123" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C123" t="s">
+        <v>276</v>
+      </c>
+    </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="7" t="s">
+      <c r="B124" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C124" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B126" s="3" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
-      <c r="B125" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
-      <c r="B126" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="1"/>
       <c r="B127" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="1"/>
       <c r="B128" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="1"/>
       <c r="B129" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" s="1"/>
+      <c r="B130" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" s="1"/>
+      <c r="B131" s="3" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
-      <c r="B130" s="46" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
-      <c r="B131" s="46" t="s">
-        <v>443</v>
       </c>
     </row>
     <row r="132" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="46" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
     </row>
     <row r="133" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="46" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
     </row>
     <row r="134" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="46" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1"/>
+      <c r="B135" s="46" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1"/>
+      <c r="B136" s="46" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="7" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="1"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B136" s="3" t="s">
+      <c r="B138" s="3" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B137" s="3" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B138" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>35</v>
+        <v>423</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>73</v>
+        <v>39</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B146" s="3" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B147" s="3" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B148" s="3" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B149" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B150" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B151" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A151" s="7" t="s">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="B151" s="5" t="s">
+      <c r="B153" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C151" t="s">
+      <c r="C153" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B152" s="3" t="s">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B154" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="3" t="s">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B155" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -5882,17 +5894,17 @@
   <hyperlinks>
     <hyperlink ref="B4" location="FailureMechanismSection" display="Sections"/>
     <hyperlink ref="B9" location="RingtoetsPipingSurfaceLine" display="SurfaceLines"/>
-    <hyperlink ref="B34" location="StochasticSoilProfile" display="StochasticSoilProfiles"/>
+    <hyperlink ref="B36" location="StochasticSoilProfile" display="StochasticSoilProfiles"/>
     <hyperlink ref="B10" location="StochasticSoilModel" display="StochasticSoilModels"/>
-    <hyperlink ref="B44" location="PipingSoilLayer" display="Layers"/>
-    <hyperlink ref="B39" location="PipingSoilProfile" display="SoilProfile"/>
+    <hyperlink ref="B46" location="PipingSoilLayer" display="Layers"/>
+    <hyperlink ref="B41" location="PipingSoilProfile" display="SoilProfile"/>
     <hyperlink ref="B11" location="GeneralPipingInput" display="GeneralInput"/>
     <hyperlink ref="B12" location="PipingProbabilityAssessmentInput" display="PipingProbabilityAssessmentInput"/>
     <hyperlink ref="B13" location="CalculationGroup" display="CalculationsGroup"/>
     <hyperlink ref="C13" location="PipingCalculationScenario" display="Contains PipingCalculationScenario"/>
-    <hyperlink ref="B75" location="PipingInput" display="InputParameters"/>
-    <hyperlink ref="B76" location="PipingOutput" display="Output"/>
-    <hyperlink ref="B77" location="PipingSemiProbabilisticOutput" display="SemiProbabilisticOutput"/>
+    <hyperlink ref="B77" location="PipingInput" display="InputParameters"/>
+    <hyperlink ref="B78" location="PipingOutput" display="Output"/>
+    <hyperlink ref="B79" location="PipingSemiProbabilisticOutput" display="SemiProbabilisticOutput"/>
     <hyperlink ref="B14" location="PipingFailureMechanismSectionResult" display="SectionResults"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added id's to datamodel Related to Issue [WTI-1092]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@8505 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: d43f5627ba2c5a54a12da9851a107800999c7931
Former-commit-id: ae48bfa3d4bf0f97de7974f64a181963a28599c4
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="8250" tabRatio="1000" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12765" tabRatio="1000" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -31,14 +31,14 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Piping!$B$156:$D$156</definedName>
     <definedName name="AssessmentSection">General!$A$5</definedName>
-    <definedName name="BreakWater">General!$A$77</definedName>
+    <definedName name="BreakWater">General!$A$78</definedName>
     <definedName name="CalculationGroup">General!$A$59</definedName>
     <definedName name="ClosingStructure">ClosingStructures!$A$29</definedName>
     <definedName name="ClosingStructureFailureMechanism">ClosingStructures!$A$1</definedName>
     <definedName name="ClosingStructureFailureMechanismSectionResult">ClosingStructures!$A$15</definedName>
     <definedName name="ClosingStructuresCalculation">ClosingStructures!$A$57</definedName>
     <definedName name="ClosingStructuresInput">ClosingStructures!$A$63</definedName>
-    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$60</definedName>
+    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$61</definedName>
     <definedName name="DikeProfile">GrassCoverErosionInwards!$A$22</definedName>
     <definedName name="DuneErosionFailureMechanism">DuneErosion!$A$1</definedName>
     <definedName name="DuneErosionFailureMechanismSectionResult">DuneErosion!$A$13</definedName>
@@ -56,11 +56,11 @@
     <definedName name="GeneralStabilityCoverWaveConditionsInput">StabilityStoneCover!$A$14</definedName>
     <definedName name="GeneralStabilityPointStructuresInput">StabilityPointStructures!$A$21</definedName>
     <definedName name="GeneralWaveImpactAsphaltCoverWaveConditionsInput">WaveImpactAsphalt!$A$28</definedName>
-    <definedName name="GrassCoverErosionInwardsCalculation">GrassCoverErosionInwards!$A$35</definedName>
+    <definedName name="GrassCoverErosionInwardsCalculation">GrassCoverErosionInwards!$A$36</definedName>
     <definedName name="GrassCoverErosionInwardsFailureMechanism">GrassCoverErosionInwards!$A$1</definedName>
-    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$67</definedName>
-    <definedName name="GrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$41</definedName>
-    <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$54</definedName>
+    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$68</definedName>
+    <definedName name="GrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$42</definedName>
+    <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$55</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanism">GrassCoverErosionOutwards!$A$1</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanismSectionResult">GrassCoverErosionOutwards!$A$24</definedName>
     <definedName name="GrassCoverErosionOutwardsHydraulicBoundaryLocation">GrassCoverErosionOutwards!$A$15</definedName>
@@ -98,7 +98,7 @@
     <definedName name="ProbabilityAssessmentOutput">General!$A$63</definedName>
     <definedName name="ReferenceLine">General!$A$32</definedName>
     <definedName name="RingtoetsPipingSurfaceLine">Piping!$A$16</definedName>
-    <definedName name="RoughnessPoint">GrassCoverErosionInwards!$A$32</definedName>
+    <definedName name="RoughnessPoint">GrassCoverErosionInwards!$A$33</definedName>
     <definedName name="StabilityPointStructure">StabilityPointStructures!$A$98</definedName>
     <definedName name="StabilityPointStructuresCalculation">StabilityPointStructures!$A$33</definedName>
     <definedName name="StabilityPointStructuresInput">StabilityPointStructures!$A$39</definedName>
@@ -115,19 +115,19 @@
     <definedName name="TechnicalInnovationFailureMechanismSectionResult">TechnicalInnovation!$A$11</definedName>
     <definedName name="WaterPressureAsphaltCoverFailureMechanism">WaterPressureAsphaltCover!$A$1</definedName>
     <definedName name="WaterPressureAsphaltCoverFailureMechanismSectionResult">WaterPressureAsphaltCover!$A$11</definedName>
-    <definedName name="WaveConditionsInput">General!$A$80</definedName>
-    <definedName name="WaveConditionsOutput">General!$A$94</definedName>
+    <definedName name="WaveConditionsInput">General!$A$81</definedName>
+    <definedName name="WaveConditionsOutput">General!$A$95</definedName>
     <definedName name="WaveImpactAsphaltCoverFailureMechanism">WaveImpactAsphalt!$A$1</definedName>
     <definedName name="WaveImpactAsphaltCoverFailureMechanismSectionResult">WaveImpactAsphalt!$A$14</definedName>
     <definedName name="WaveImpactAsphaltCoverWaveConditionsOutput">WaveImpactAsphalt!$A$25</definedName>
-    <definedName name="WmtsMapData">General!$A$105</definedName>
+    <definedName name="WmtsMapData">General!$A$106</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="469">
   <si>
     <t>Description</t>
   </si>
@@ -1072,9 +1072,6 @@
   </si>
   <si>
     <t>per failuremechanism</t>
-  </si>
-  <si>
-    <t>WTI-851</t>
   </si>
   <si>
     <t>GeneralStabilityStoneCoverWaveConditionsInput</t>
@@ -1665,7 +1662,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
@@ -1717,6 +1714,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
@@ -2117,17 +2115,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2229,17 +2227,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="29" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2341,17 +2339,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="31" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2453,17 +2451,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="33" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,17 +2563,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="35" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="35" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="32" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="35" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2677,17 +2675,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="37" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="37" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="37" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2725,7 +2723,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>307</v>
@@ -2737,7 +2735,7 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C15" t="s">
         <v>118</v>
@@ -2918,17 +2916,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="39" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="39" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="39" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2992,7 +2990,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -3024,17 +3022,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="41" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="41" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="41" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3044,13 +3042,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -3072,15 +3070,15 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>278</v>
@@ -3088,18 +3086,18 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>229</v>
       </c>
       <c r="C15" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>262</v>
@@ -3122,7 +3120,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
@@ -3141,7 +3139,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C23" t="s">
         <v>118</v>
@@ -3149,7 +3147,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C24" t="s">
         <v>118</v>
@@ -3157,7 +3155,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C25" t="s">
         <v>118</v>
@@ -3165,7 +3163,7 @@
     </row>
     <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -3173,7 +3171,7 @@
     </row>
     <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
@@ -3181,7 +3179,7 @@
     </row>
     <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C28" t="s">
         <v>118</v>
@@ -3189,7 +3187,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C29" t="s">
         <v>118</v>
@@ -3197,7 +3195,7 @@
     </row>
     <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
@@ -3205,7 +3203,7 @@
     </row>
     <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C31" t="s">
         <v>118</v>
@@ -3213,18 +3211,18 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>156</v>
@@ -3251,7 +3249,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>112</v>
@@ -3259,7 +3257,7 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>281</v>
@@ -3268,46 +3266,46 @@
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -3317,7 +3315,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C50" t="s">
         <v>118</v>
@@ -3325,12 +3323,12 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C52" t="s">
         <v>118</v>
@@ -3338,17 +3336,17 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C55" t="s">
         <v>118</v>
@@ -3356,12 +3354,12 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C57" s="44" t="s">
         <v>118</v>
@@ -3369,132 +3367,132 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
@@ -3504,7 +3502,7 @@
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
@@ -3524,47 +3522,47 @@
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>1</v>
@@ -3572,7 +3570,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>3</v>
@@ -3585,7 +3583,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -3595,47 +3593,47 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -3645,7 +3643,7 @@
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
@@ -3660,117 +3658,117 @@
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C138" s="44" t="s">
         <v>118</v>
@@ -3778,42 +3776,42 @@
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>44</v>
@@ -3821,7 +3819,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>45</v>
@@ -3923,17 +3921,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="43" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="43" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="43" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4029,17 +4027,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4090,10 +4088,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E77" sqref="E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4257,10 +4255,10 @@
     </row>
     <row r="30" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -4328,7 +4326,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4336,52 +4334,52 @@
         <v>272</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="14"/>
       <c r="B46" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="B49" s="46" t="s">
         <v>433</v>
-      </c>
-      <c r="B49" s="46" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="46" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="46" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="46" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="46" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4456,235 +4454,239 @@
       <c r="A69" s="46" t="s">
         <v>281</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="48"/>
+      <c r="B70" s="46" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="8" t="s">
-        <v>315</v>
-      </c>
-      <c r="B70" s="46" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="8"/>
+      <c r="B71" s="46" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="46" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B72" s="46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="46" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="9" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="5" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C74" t="s">
+      <c r="C75" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="46" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="46" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B78" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="3" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>284</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B81" s="11" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>314</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B82" s="11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="5" t="s">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B83" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="11" t="s">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B84" s="11" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C85" t="s">
-        <v>286</v>
+        <v>50</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B86" s="5" t="s">
-        <v>296</v>
+        <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
+      </c>
+      <c r="C87" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>292</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B95" s="5" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>314</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B96" s="5" t="s">
         <v>272</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="5" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
-        <v>427</v>
+        <v>295</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="46" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="46" t="s">
+        <v>458</v>
+      </c>
+      <c r="B106" s="46" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="8"/>
+      <c r="B107" s="46" t="s">
         <v>459</v>
-      </c>
-      <c r="B105" s="46" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="8"/>
-      <c r="B106" s="46" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B107" s="46" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B108" s="46" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B109" s="46" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B110" s="46" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B111" s="46" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="5" t="s">
+      <c r="C112" t="s">
         <v>464</v>
-      </c>
-      <c r="C111" t="s">
-        <v>465</v>
       </c>
     </row>
   </sheetData>
@@ -4715,18 +4717,17 @@
     <hyperlink ref="B18" location="WaveImpactAsphaltCoverFailureMechanism" display="WaveImpactAsphaltCover"/>
     <hyperlink ref="B23" location="HeightStructuresFailureMechanism" display="HeightStructures"/>
     <hyperlink ref="B3" location="AssessmentSection" display="AssessmentSections"/>
-    <hyperlink ref="B73" location="BreakWater" display="BreakWater"/>
-    <hyperlink ref="B80" location="ForeshoreProfile" display="ForeshoreProfile"/>
-    <hyperlink ref="B81" location="HydraulicBoundaryLocation" display="HydraulicBoundaryLocation"/>
-    <hyperlink ref="B83" location="BreakWater" display="BreakWater"/>
-    <hyperlink ref="A70" r:id="rId1" tooltip="View this issue in JIRA" display="https://issuetracker.deltares.nl/browse/WTI-851"/>
+    <hyperlink ref="B74" location="BreakWater" display="BreakWater"/>
+    <hyperlink ref="B81" location="ForeshoreProfile" display="ForeshoreProfile"/>
+    <hyperlink ref="B82" location="HydraulicBoundaryLocation" display="HydraulicBoundaryLocation"/>
+    <hyperlink ref="B84" location="BreakWater" display="BreakWater"/>
     <hyperlink ref="B46" location="HydraulicBoundaryLocationOutput" display="DesignWaterLevelOutput"/>
     <hyperlink ref="B47" location="HydraulicBoundaryLocationOutput" display="WaveHeightOutput"/>
     <hyperlink ref="B30" location="WmtsMapData" display="BackgroundMapData"/>
-    <hyperlink ref="C30" r:id="rId2"/>
+    <hyperlink ref="C30" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4780,17 +4781,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="46" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="46" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="46" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4898,7 +4899,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>54</v>
@@ -4917,7 +4918,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
@@ -4944,7 +4945,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
@@ -4990,17 +4991,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5116,19 +5117,19 @@
     </row>
     <row r="28" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>456</v>
+      </c>
+      <c r="B28" s="46" t="s">
         <v>457</v>
-      </c>
-      <c r="B28" s="46" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B30" s="46" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5203,17 +5204,17 @@
         <v>130</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
         <v>20</v>
       </c>
@@ -5259,12 +5260,12 @@
         <v>265</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>267</v>
       </c>
@@ -5499,7 +5500,7 @@
     </row>
     <row r="95" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="46" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -5763,31 +5764,31 @@
     <row r="132" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="46" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="133" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="46" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="134" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="46" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="135" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="46" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="136" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="46" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -5803,7 +5804,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -5915,10 +5916,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C71"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5962,17 +5963,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="17" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6065,322 +6066,329 @@
         <v>118</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" s="44" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="46" t="s">
         <v>1</v>
-      </c>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B23" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B26" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B26" s="5" t="s">
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B27" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C27" s="8"/>
-    </row>
-    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B29" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B29" s="9" t="s">
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B30" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B30" s="3" t="s">
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B31" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A32" s="7" t="s">
+      <c r="C31" s="8"/>
+    </row>
+    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B33" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="C32" s="8"/>
-    </row>
-    <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B33" s="3" t="s">
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B34" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="8"/>
-    </row>
-    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+      <c r="C34" s="8"/>
+    </row>
+    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B36" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="C35" s="8"/>
-    </row>
-    <row r="36" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="9" t="s">
-        <v>11</v>
       </c>
       <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="3" t="s">
-        <v>10</v>
+      <c r="B37" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="3" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
-      <c r="B39" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C39" t="s">
-        <v>157</v>
-      </c>
+      <c r="B39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="8"/>
     </row>
     <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
+      <c r="B40" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="C40" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="1"/>
+    </row>
+    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C41" s="8"/>
-    </row>
-    <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="3" t="s">
+      <c r="C42" s="8"/>
+    </row>
+    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="8"/>
-    </row>
-    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="8"/>
+    </row>
+    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="8"/>
-    </row>
-    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B44" s="9" t="s">
+      <c r="C44" s="8"/>
+    </row>
+    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B45" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="C44" s="8"/>
-    </row>
-    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B45" s="3" t="s">
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="8"/>
-    </row>
-    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B46" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" t="s">
-        <v>210</v>
-      </c>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B47" s="5" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B48" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C48" s="8"/>
+      <c r="B48" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B49" s="3" t="s">
-        <v>208</v>
+        <v>51</v>
       </c>
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B50" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B51" s="3" t="s">
-        <v>112</v>
+        <v>209</v>
       </c>
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B52" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B53" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="C52" s="8"/>
-    </row>
-    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A54" s="7" t="s">
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B55" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="8"/>
-    </row>
-    <row r="55" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="9" t="s">
-        <v>445</v>
-      </c>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="B56" s="3" t="s">
+    <row r="56" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="B57" s="3" t="s">
         <v>271</v>
-      </c>
-      <c r="C56" s="8"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
-        <v>272</v>
       </c>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C58" s="8"/>
-    </row>
-    <row r="60" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
-        <v>445</v>
-      </c>
-      <c r="B60" s="46" t="s">
+      <c r="C59" s="8"/>
+    </row>
+    <row r="61" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="B61" s="46" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B61" s="46" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="62" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="46" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="46" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="46" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="46" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="46" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B68" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C68" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B68" s="3" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C68" s="8"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="5" t="s">
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C70" t="s">
         <v>213</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
         <v>188</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" location="FailureMechanismSection" display="Sections"/>
-    <hyperlink ref="B27" location="BreakWater" display="BreakWater"/>
-    <hyperlink ref="B29" location="RoughnessPoint" display="DikeGeometry"/>
+    <hyperlink ref="B28" location="BreakWater" display="BreakWater"/>
+    <hyperlink ref="B30" location="RoughnessPoint" display="DikeGeometry"/>
     <hyperlink ref="B10" location="DikeProfile" display="DikeProfiles"/>
     <hyperlink ref="B11" location="CalculationGroup" display="CalculationsGroup"/>
     <hyperlink ref="C11" location="GrassCoverErosionInwardsCalculation" display="Contains GrassCoverErosionInwardsCalculation"/>
-    <hyperlink ref="B35" location="GrassCoverErosionInwardsInput" display="InputParameters"/>
-    <hyperlink ref="B44" location="BreakWater" display="BreakWater"/>
-    <hyperlink ref="B36" location="GrassCoverErosionInwardsOutput" display="Output"/>
+    <hyperlink ref="B36" location="GrassCoverErosionInwardsInput" display="InputParameters"/>
+    <hyperlink ref="B45" location="BreakWater" display="BreakWater"/>
+    <hyperlink ref="B37" location="GrassCoverErosionInwardsOutput" display="Output"/>
     <hyperlink ref="B12" location="GrassCoverErosionInwardsFailureMechanismSectionResult" display="SectionResults"/>
-    <hyperlink ref="B54" location="ProbabilityAssessmentOutput" display="ProbabilityAssessmentOutput"/>
+    <hyperlink ref="B55" location="ProbabilityAssessmentOutput" display="ProbabilityAssessmentOutput"/>
     <hyperlink ref="B9" location="GeneralGrassCoverErosionInwardsInput" display="GeneralInput"/>
-    <hyperlink ref="B55" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
+    <hyperlink ref="B56" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -6392,8 +6400,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6438,17 +6446,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6486,7 +6494,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>100</v>
@@ -6494,7 +6502,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>278</v>
@@ -6502,7 +6510,7 @@
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
@@ -6510,7 +6518,7 @@
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>3</v>
@@ -6523,17 +6531,17 @@
     </row>
     <row r="18" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
@@ -6553,22 +6561,22 @@
     </row>
     <row r="24" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
@@ -6578,17 +6586,17 @@
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6620,7 +6628,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C36" t="s">
         <v>118</v>
@@ -6628,7 +6636,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C37" t="s">
         <v>118</v>
@@ -6692,17 +6700,17 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C49" t="s">
         <v>118</v>
@@ -6715,7 +6723,7 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C51" t="s">
         <v>118</v>
@@ -6723,22 +6731,22 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
@@ -6748,7 +6756,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
@@ -6768,32 +6776,32 @@
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6835,7 +6843,7 @@
         <v>262</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6858,7 +6866,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>44</v>
@@ -6924,8 +6932,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B95" sqref="B95"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6938,7 +6946,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -6970,17 +6978,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="19" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6990,13 +6998,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7017,15 +7025,15 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>278</v>
@@ -7033,13 +7041,13 @@
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>229</v>
       </c>
       <c r="C15" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -7047,7 +7055,7 @@
         <v>262</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -7070,10 +7078,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C21" t="s">
         <v>118</v>
@@ -7084,7 +7092,7 @@
         <v>312</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -7105,7 +7113,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C25" t="s">
         <v>118</v>
@@ -7113,7 +7121,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -7121,7 +7129,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
@@ -7137,7 +7145,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>3</v>
@@ -7152,7 +7160,7 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7164,79 +7172,79 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -7248,7 +7256,7 @@
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -7266,53 +7274,53 @@
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -7335,7 +7343,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>112</v>
@@ -7343,7 +7351,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>281</v>
@@ -7351,57 +7359,57 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C75" t="s">
         <v>118</v>
@@ -7409,12 +7417,12 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C77" t="s">
         <v>118</v>
@@ -7422,52 +7430,52 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
@@ -7492,22 +7500,22 @@
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
@@ -7525,12 +7533,12 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>44</v>
@@ -7538,7 +7546,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>45</v>
@@ -7642,17 +7650,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7670,7 +7678,7 @@
     </row>
     <row r="10" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="47" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -7707,7 +7715,7 @@
     <row r="17" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="46" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B18" s="46" t="s">
         <v>56</v>
@@ -7718,7 +7726,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="46" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B21" s="46" t="s">
         <v>3</v>
@@ -7737,12 +7745,12 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="46" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="46" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7752,7 +7760,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="46" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -7762,7 +7770,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B30" s="46" t="s">
         <v>293</v>
@@ -7776,32 +7784,32 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="46" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="46" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="46" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="46" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="46" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="46" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -7868,19 +7876,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="23" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="23" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7946,7 +7954,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -7955,19 +7963,19 @@
         <v>272</v>
       </c>
       <c r="C19" s="44" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
       <c r="B21" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -8018,7 +8026,7 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C31" t="s">
         <v>118</v>
@@ -8081,7 +8089,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
   </sheetData>
@@ -8154,17 +8162,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated database model so that Id is added to DikeProfileEntity and ForeshoreProfileEntity. Id is required and Name is now also required for a ForeshoreProfile. Related to Issue [WTI-1092]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@8538 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 3df4ed85c2de927f7703910090b721b49d593e5a
Former-commit-id: d300debe30d6f69ea3b99bcbae64bfecd30e3922
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12765" tabRatio="1000" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -4090,8 +4090,8 @@
   </sheetPr>
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4454,7 +4454,7 @@
       <c r="A69" s="46" t="s">
         <v>281</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B69" s="46" t="s">
         <v>3</v>
       </c>
     </row>
@@ -5918,8 +5918,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6070,7 +6070,7 @@
       <c r="A22" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="46" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="8"/>
@@ -6223,7 +6223,7 @@
       </c>
       <c r="C46" s="8"/>
     </row>
-    <row r="47" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="5" t="s">
         <v>84</v>
       </c>
@@ -6231,7 +6231,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="5" t="s">
         <v>83</v>
       </c>
@@ -6239,40 +6239,40 @@
         <v>210</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C49" s="8"/>
     </row>
-    <row r="50" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>208</v>
       </c>
       <c r="C50" s="8"/>
     </row>
-    <row r="51" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>209</v>
       </c>
       <c r="C51" s="8"/>
     </row>
-    <row r="52" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>112</v>
       </c>
       <c r="C52" s="8"/>
     </row>
-    <row r="53" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>273</v>
       </c>
       <c r="C53" s="8"/>
     </row>
-    <row r="54" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>270</v>
       </c>
@@ -6287,7 +6287,7 @@
       </c>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>271</v>
       </c>

</xml_diff>

<commit_message>
Addes Type column to Stochastic Soil Profile, which can have a value of 1 or 2 (1D or 2D). Related to Issue [WTI-1191]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@8597 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 2ecf66645a7b85ca78e884bf37a4cb25a11344d9
Former-commit-id: ce4b36dd0ab58d44dd0195b60f504a370db7642a
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="469">
   <si>
     <t>Description</t>
   </si>
@@ -4945,8 +4945,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5164,15 +5164,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="46" t="s">
         <v>17</v>
-      </c>
-      <c r="C38" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -5918,7 +5915,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated OpslagMapping.xlsx Related to Issue [WTI-1141]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@8696 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 9c28bab175c66ce01201bd25dd1b52b008979c83
Former-commit-id: d5181f336d26c4166a304ea4f8fc7d733da8e65c
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -31,6 +31,8 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Piping!$B$156:$D$156</definedName>
     <definedName name="AssessmentSection">General!$A$5</definedName>
+    <definedName name="BackgroundData">General!$A$106</definedName>
+    <definedName name="BackgroundDataMeta">General!$A$113</definedName>
     <definedName name="BreakWater">General!$A$78</definedName>
     <definedName name="CalculationGroup">General!$A$59</definedName>
     <definedName name="ClosingStructure">ClosingStructures!$A$29</definedName>
@@ -120,7 +122,6 @@
     <definedName name="WaveImpactAsphaltCoverFailureMechanism">WaveImpactAsphalt!$A$1</definedName>
     <definedName name="WaveImpactAsphaltCoverFailureMechanismSectionResult">WaveImpactAsphalt!$A$14</definedName>
     <definedName name="WaveImpactAsphaltCoverWaveConditionsOutput">WaveImpactAsphalt!$A$25</definedName>
-    <definedName name="WmtsMapData">General!$A$106</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1503,37 +1504,37 @@
     <t>SourcePath</t>
   </si>
   <si>
-    <t>BackgroundMapData</t>
-  </si>
-  <si>
     <t>IsVisible</t>
   </si>
   <si>
-    <t>SourceCapabilitiesUrl</t>
-  </si>
-  <si>
-    <t>SelectedCapabilityName</t>
-  </si>
-  <si>
     <t>Transparency</t>
   </si>
   <si>
     <t>IsConfigured</t>
   </si>
   <si>
-    <t>Derived from internal state</t>
-  </si>
-  <si>
-    <t>WTI-1087</t>
-  </si>
-  <si>
     <t>FlowVelocityStructureClosable.CoefficientOfVariation</t>
   </si>
   <si>
-    <t>PreferredFormat</t>
-  </si>
-  <si>
     <t>SurfaceLineCollection</t>
+  </si>
+  <si>
+    <t>BackgroundData</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>BackgroundMapDataType</t>
+  </si>
+  <si>
+    <t>BackgroundDataMeta</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1663,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
@@ -1675,7 +1676,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -2114,17 +2114,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="26" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+    <row r="6" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="26" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="27" t="s">
+    <row r="7" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="26" t="s">
         <v>425</v>
       </c>
     </row>
@@ -2226,17 +2226,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="29" t="s">
+    <row r="6" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+    <row r="7" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
         <v>425</v>
       </c>
     </row>
@@ -2338,17 +2338,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+    <row r="6" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="30" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
+    <row r="7" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
         <v>425</v>
       </c>
     </row>
@@ -2450,17 +2450,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="32" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="33" t="s">
+    <row r="6" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="32" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="33" t="s">
+    <row r="7" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="32" t="s">
         <v>425</v>
       </c>
     </row>
@@ -2562,17 +2562,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+    <row r="6" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+    <row r="7" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34" t="s">
         <v>425</v>
       </c>
     </row>
@@ -2674,17 +2674,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+    <row r="6" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+    <row r="7" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="36" t="s">
         <v>425</v>
       </c>
     </row>
@@ -2710,7 +2710,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="9" t="s">
         <v>282</v>
       </c>
@@ -2915,17 +2915,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="38" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="38" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
+    <row r="7" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="38" t="s">
         <v>425</v>
       </c>
     </row>
@@ -3021,17 +3021,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41" t="s">
+    <row r="6" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="40" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41" t="s">
+    <row r="7" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40" t="s">
         <v>425</v>
       </c>
     </row>
@@ -3359,9 +3359,9 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="C57" s="44" t="s">
+        <v>461</v>
+      </c>
+      <c r="C57" s="43" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3768,9 +3768,9 @@
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="C138" s="44" t="s">
+        <v>461</v>
+      </c>
+      <c r="C138" s="43" t="s">
         <v>118</v>
       </c>
     </row>
@@ -3920,17 +3920,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="42" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
+    <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="40" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="43" t="s">
+    <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
         <v>425</v>
       </c>
     </row>
@@ -4026,17 +4026,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="44" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="45" t="s">
+    <row r="6" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="44" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="45" t="s">
+    <row r="7" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44" t="s">
         <v>425</v>
       </c>
     </row>
@@ -4088,10 +4088,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C112"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4253,13 +4253,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
-        <v>458</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>465</v>
-      </c>
+    <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="C30" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
@@ -4333,56 +4331,56 @@
       <c r="B45" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="C45" s="44" t="s">
+      <c r="C45" s="43" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+    <row r="46" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
       <c r="B46" s="9" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+    <row r="47" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
       <c r="B47" s="9" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>432</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="45" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="46" t="s">
+    <row r="50" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="45" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="46" t="s">
+    <row r="51" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="45" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="46" t="s">
+    <row r="52" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="45" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="46" t="s">
+    <row r="53" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="45" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="46" t="s">
+    <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="45" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>117</v>
@@ -4451,32 +4449,32 @@
       <c r="C67" s="8"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="46" t="s">
+      <c r="A69" s="45" t="s">
         <v>281</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="48"/>
-      <c r="B70" s="46" t="s">
+    <row r="70" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="47"/>
+      <c r="B70" s="45" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
-      <c r="B71" s="46" t="s">
+      <c r="B71" s="45" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="46" t="s">
+      <c r="B72" s="45" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="46" t="s">
+      <c r="B73" s="45" t="s">
         <v>49</v>
       </c>
     </row>
@@ -4494,7 +4492,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="46" t="s">
+      <c r="B76" s="45" t="s">
         <v>14</v>
       </c>
     </row>
@@ -4607,87 +4605,98 @@
         <v>272</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="46" t="s">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="45" t="s">
+        <v>463</v>
+      </c>
+      <c r="B106" s="45" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="8"/>
+      <c r="B107" s="45" t="s">
         <v>458</v>
       </c>
-      <c r="B106" s="46" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="8"/>
-      <c r="B107" s="46" t="s">
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="45" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B108" s="46" t="s">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="45" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B110" s="45" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B109" s="46" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B110" s="46" t="s">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="43"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="45" t="s">
+        <v>466</v>
+      </c>
+      <c r="B113" s="45" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B111" s="46" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B112" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="C112" t="s">
-        <v>464</v>
-      </c>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="45" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="43"/>
     </row>
   </sheetData>
   <sortState ref="B82:C85">
@@ -4723,11 +4732,11 @@
     <hyperlink ref="B84" location="BreakWater" display="BreakWater"/>
     <hyperlink ref="B46" location="HydraulicBoundaryLocationOutput" display="DesignWaterLevelOutput"/>
     <hyperlink ref="B47" location="HydraulicBoundaryLocationOutput" display="WaveHeightOutput"/>
-    <hyperlink ref="B30" location="WmtsMapData" display="BackgroundMapData"/>
-    <hyperlink ref="C30" r:id="rId1"/>
+    <hyperlink ref="B111" location="BackgroundDataMeta" display="Parameters"/>
+    <hyperlink ref="B30" location="BackgroundData" display="BackgroundData"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4780,17 +4789,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+    <row r="6" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+    <row r="7" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="45" t="s">
         <v>425</v>
       </c>
     </row>
@@ -4863,7 +4872,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="9" t="s">
         <v>11</v>
       </c>
@@ -4945,7 +4954,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -4990,17 +4999,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>425</v>
       </c>
     </row>
@@ -5112,23 +5121,23 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="48"/>
-    </row>
-    <row r="28" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="47"/>
+    </row>
+    <row r="28" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="45" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>468</v>
-      </c>
-      <c r="B30" s="46" t="s">
+        <v>462</v>
+      </c>
+      <c r="B30" s="45" t="s">
         <v>457</v>
       </c>
     </row>
@@ -5168,7 +5177,7 @@
       <c r="A38" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="46" t="s">
+      <c r="B38" s="45" t="s">
         <v>17</v>
       </c>
     </row>
@@ -5283,19 +5292,19 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="46" t="s">
+      <c r="A61" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="D61" s="44"/>
+      <c r="D61" s="43"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B62" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C62" s="44" t="s">
+      <c r="C62" s="43" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5303,7 +5312,7 @@
       <c r="B63" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C63" s="44" t="s">
+      <c r="C63" s="43" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5491,12 +5500,12 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="46" t="s">
+      <c r="B94" s="45" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="95" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="46" t="s">
+    <row r="95" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="45" t="s">
         <v>440</v>
       </c>
     </row>
@@ -5758,33 +5767,33 @@
         <v>40</v>
       </c>
     </row>
-    <row r="132" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
-      <c r="B132" s="46" t="s">
+      <c r="B132" s="45" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="133" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
-      <c r="B133" s="46" t="s">
+      <c r="B133" s="45" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="134" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
-      <c r="B134" s="46" t="s">
+      <c r="B134" s="45" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="135" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
-      <c r="B135" s="46" t="s">
+      <c r="B135" s="45" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="136" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
-      <c r="B136" s="46" t="s">
+      <c r="B136" s="45" t="s">
         <v>439</v>
       </c>
     </row>
@@ -5959,17 +5968,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>423</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>424</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>425</v>
       </c>
     </row>
@@ -6067,14 +6076,14 @@
       <c r="A22" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="45" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" s="44" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A23" s="49"/>
-      <c r="B23" s="46" t="s">
+    <row r="23" spans="1:3" s="43" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+      <c r="A23" s="48"/>
+      <c r="B23" s="45" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="8"/>
@@ -6195,26 +6204,26 @@
       </c>
       <c r="C42" s="8"/>
     </row>
-    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C43" s="8"/>
     </row>
-    <row r="44" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>52</v>
       </c>
       <c r="C44" s="8"/>
     </row>
-    <row r="45" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
         <v>82</v>
       </c>
       <c r="C45" s="8"/>
     </row>
-    <row r="46" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>50</v>
       </c>
@@ -6278,7 +6287,7 @@
       </c>
       <c r="C55" s="8"/>
     </row>
-    <row r="56" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
         <v>444</v>
       </c>
@@ -6302,40 +6311,40 @@
       </c>
       <c r="C59" s="8"/>
     </row>
-    <row r="61" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="62" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="46" t="s">
+    <row r="62" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="45" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="46" t="s">
+    <row r="63" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="45" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="46" t="s">
+    <row r="64" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="45" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="46" t="s">
+    <row r="65" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="45" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="46" t="s">
+    <row r="66" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="45" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>196</v>
@@ -6974,17 +6983,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="19" t="s">
+    <row r="6" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="19" t="s">
+    <row r="7" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
         <v>425</v>
       </c>
     </row>
@@ -7646,17 +7655,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+    <row r="6" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+    <row r="7" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
         <v>425</v>
       </c>
     </row>
@@ -7673,12 +7682,12 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="47" t="s">
+    <row r="10" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="46" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="11" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
@@ -7709,103 +7718,103 @@
         <v>189</v>
       </c>
     </row>
-    <row r="17" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+    <row r="17" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="45" t="s">
         <v>453</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="46" t="s">
+      <c r="A21" s="45" t="s">
         <v>449</v>
       </c>
-      <c r="B21" s="46" t="s">
+      <c r="B21" s="45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="45" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="46" t="s">
+      <c r="B23" s="45" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
+      <c r="B24" s="45" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="46" t="s">
+      <c r="B25" s="45" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" s="46" t="s">
+      <c r="B26" s="45" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" s="46" t="s">
+      <c r="B27" s="45" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="28" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="46" t="s">
+    <row r="28" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="45" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="46" t="s">
+      <c r="A30" s="45" t="s">
         <v>454</v>
       </c>
-      <c r="B30" s="46" t="s">
+      <c r="B30" s="45" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
-      <c r="B31" s="46" t="s">
+      <c r="B31" s="45" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="46" t="s">
+      <c r="B32" s="45" t="s">
         <v>455</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="46" t="s">
+      <c r="B33" s="45" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="46" t="s">
+      <c r="B34" s="45" t="s">
         <v>428</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="45" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="46" t="s">
+      <c r="B36" s="45" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="45" t="s">
         <v>431</v>
       </c>
     </row>
@@ -7872,19 +7881,19 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="22" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="22" t="s">
         <v>425</v>
       </c>
     </row>
@@ -7902,7 +7911,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="9" t="s">
         <v>282</v>
       </c>
@@ -7940,13 +7949,13 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
         <v>4</v>
       </c>
@@ -7955,22 +7964,22 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="43" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="44" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
         <v>436</v>
       </c>
@@ -8158,17 +8167,17 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="24" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
+    <row r="7" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
         <v>425</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated database design - Added extra column in GrassCoverErosionInwardsCalculationEntity - Added extra table for overtopping rate output. Related to Issue [WTI-860]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9210 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: c59221ee07a32a70e391a1b0c952169f7f13670e
Former-commit-id: faf175580b69c6c21d340bbfaae25eb3027af16d
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="ClosingStructureFailureMechanismSectionResult">ClosingStructures!$A$15</definedName>
     <definedName name="ClosingStructuresCalculation">ClosingStructures!$A$57</definedName>
     <definedName name="ClosingStructuresInput">ClosingStructures!$A$63</definedName>
-    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$61</definedName>
+    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$64</definedName>
     <definedName name="DikeProfile">GrassCoverErosionInwards!$A$22</definedName>
     <definedName name="DuneErosionFailureMechanism">DuneErosion!$A$1</definedName>
     <definedName name="DuneErosionFailureMechanismSectionResult">DuneErosion!$A$13</definedName>
@@ -60,9 +60,9 @@
     <definedName name="GeneralWaveImpactAsphaltCoverWaveConditionsInput">WaveImpactAsphalt!$A$28</definedName>
     <definedName name="GrassCoverErosionInwardsCalculation">GrassCoverErosionInwards!$A$36</definedName>
     <definedName name="GrassCoverErosionInwardsFailureMechanism">GrassCoverErosionInwards!$A$1</definedName>
-    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$68</definedName>
+    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$78</definedName>
     <definedName name="GrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$42</definedName>
-    <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$55</definedName>
+    <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$57</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanism">GrassCoverErosionOutwards!$A$1</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanismSectionResult">GrassCoverErosionOutwards!$A$24</definedName>
     <definedName name="GrassCoverErosionOutwardsHydraulicBoundaryLocation">GrassCoverErosionOutwards!$A$15</definedName>
@@ -86,6 +86,7 @@
     <definedName name="MacrostabilityOutwardsFailureMechanismSectionResult">MacrostabilityOutwards!$A$11</definedName>
     <definedName name="MicrostabilityFailureMechanism">Microstability!$A$1</definedName>
     <definedName name="MicrostabilityFailureMechanismSectionResult">Microstability!$A$11</definedName>
+    <definedName name="OvertoppingRateAssessmentOutput">GrassCoverErosionInwards!$A$71</definedName>
     <definedName name="PipingCalculationScenario">Piping!$A$77</definedName>
     <definedName name="PipingFailureMechanism">Piping!$A$1</definedName>
     <definedName name="PipingFailureMechanismSectionResult">Piping!$A$153</definedName>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1217" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="473">
   <si>
     <t>Description</t>
   </si>
@@ -1535,6 +1536,18 @@
   </si>
   <si>
     <t>Value</t>
+  </si>
+  <si>
+    <t>DikeHeightCalculationType</t>
+  </si>
+  <si>
+    <t>OvertoppingRateCalculationType</t>
+  </si>
+  <si>
+    <t>OvertoppingRateAssessmentOutput</t>
+  </si>
+  <si>
+    <t>OvertoppingRate</t>
   </si>
 </sst>
 </file>
@@ -4090,8 +4103,8 @@
   </sheetPr>
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5922,10 +5935,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6275,108 +6288,160 @@
       </c>
       <c r="C53" s="8"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="45" t="s">
+        <v>469</v>
+      </c>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+    <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="45" t="s">
+        <v>470</v>
+      </c>
+      <c r="C55" s="8"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>270</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B57" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="C55" s="8"/>
-    </row>
-    <row r="56" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="9" t="s">
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="C56" s="8"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+      <c r="C58" s="8"/>
+    </row>
+    <row r="59" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="C59" s="8"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="C57" s="8"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B58" s="3" t="s">
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="C58" s="8"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B59" s="3" t="s">
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C59" s="8"/>
-    </row>
-    <row r="61" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+      <c r="C62" s="8"/>
+    </row>
+    <row r="64" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
         <v>444</v>
       </c>
-      <c r="B61" s="45" t="s">
+      <c r="B64" s="45" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="45" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="45" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="45" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="45" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="45" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="45" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="45" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="45" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+    <row r="70" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="B71" s="45" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="45" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="45" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="45" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="45" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="45" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B78" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C78" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B69" s="3" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C69" s="8"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="5" t="s">
+      <c r="C79" s="8"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C80" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="3" t="s">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="3" t="s">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="3" t="s">
         <v>188</v>
       </c>
     </row>
@@ -6392,9 +6457,10 @@
     <hyperlink ref="B45" location="BreakWater" display="BreakWater"/>
     <hyperlink ref="B37" location="GrassCoverErosionInwardsOutput" display="Output"/>
     <hyperlink ref="B12" location="GrassCoverErosionInwardsFailureMechanismSectionResult" display="SectionResults"/>
-    <hyperlink ref="B55" location="ProbabilityAssessmentOutput" display="ProbabilityAssessmentOutput"/>
+    <hyperlink ref="B57" location="ProbabilityAssessmentOutput" display="ProbabilityAssessmentOutput"/>
     <hyperlink ref="B9" location="GeneralGrassCoverErosionInwardsInput" display="GeneralInput"/>
-    <hyperlink ref="B56" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
+    <hyperlink ref="B58" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
+    <hyperlink ref="B59" location="OvertoppingRateAssessmentOutput" display="OvertoppingRateAssessmentOutput"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Merged all revision(s) from branches/UpdateDikeProfilesFeature
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9282 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 5f84130acb4bd2113b949015b4049e0c0b5795c4
Former-commit-id: 86ce2960f4b2cd6be35b62d7b6608749e29f1022
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="474">
   <si>
     <t>Description</t>
   </si>
@@ -1548,6 +1548,9 @@
   </si>
   <si>
     <t>OvertoppingRate</t>
+  </si>
+  <si>
+    <t>DikeProfileCollection</t>
   </si>
 </sst>
 </file>
@@ -5935,10 +5938,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6435,14 +6438,22 @@
         <v>213</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="45" t="s">
+        <v>473</v>
+      </c>
+      <c r="B84" s="45" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Incorporated comments review 1665: - Updated the OpslagMapping.xlsx - Cleaned files - Renamed variables Related to Issue [WTI-1238]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9319 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 0e7e699e098a938c6785ffcfb42411a4bd165220
Former-commit-id: e6d4357a4ed691736a9a5fa803b9bb1e4dc3440f
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -650,15 +650,9 @@
     <t>Diameter70.Mean</t>
   </si>
   <si>
-    <t>Diameter70.StandardDeviation</t>
-  </si>
-  <si>
     <t>DarcyPermeability.Mean</t>
   </si>
   <si>
-    <t>DarcyPermeability.StandardDeviation</t>
-  </si>
-  <si>
     <t>DampingFactorExit.Mean</t>
   </si>
   <si>
@@ -929,15 +923,9 @@
     <t>DiameterD70Mean</t>
   </si>
   <si>
-    <t>DiameterD70Deviation</t>
-  </si>
-  <si>
     <t>PermeabilityMean</t>
   </si>
   <si>
-    <t>PermeabilityDeviation</t>
-  </si>
-  <si>
     <t>BelowPhreaticLevelShift</t>
   </si>
   <si>
@@ -1551,6 +1539,18 @@
   </si>
   <si>
     <t>DikeProfileCollection</t>
+  </si>
+  <si>
+    <t>PermeabilityCoefficientOfVariation</t>
+  </si>
+  <si>
+    <t>DiameterD70CoefficientOfVariation</t>
+  </si>
+  <si>
+    <t>Diameter70.CoefficientOfVariation</t>
+  </si>
+  <si>
+    <t>DarcyPermeability.CoefficientOfVariation</t>
   </si>
 </sst>
 </file>
@@ -2071,7 +2071,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2131,17 +2131,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2154,33 +2154,33 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2243,17 +2243,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="28" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2266,33 +2266,33 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2355,17 +2355,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2378,33 +2378,33 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2467,17 +2467,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2490,33 +2490,33 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2579,17 +2579,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2602,33 +2602,33 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2691,17 +2691,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2714,7 +2714,7 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -2728,21 +2728,21 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C14" t="s">
         <v>118</v>
@@ -2751,7 +2751,7 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C15" t="s">
         <v>118</v>
@@ -2760,7 +2760,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C16" t="s">
         <v>118</v>
@@ -2769,7 +2769,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C17" t="s">
         <v>118</v>
@@ -2778,7 +2778,7 @@
     <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C18" t="s">
         <v>118</v>
@@ -2787,7 +2787,7 @@
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C19" t="s">
         <v>118</v>
@@ -2795,7 +2795,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>156</v>
@@ -2827,42 +2827,42 @@
     </row>
     <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C31" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -2900,7 +2900,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -2932,17 +2932,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2955,28 +2955,28 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -3006,7 +3006,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -3038,17 +3038,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="40" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3058,18 +3058,18 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
@@ -3081,62 +3081,62 @@
         <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
@@ -3144,10 +3144,10 @@
     </row>
     <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C22" t="s">
         <v>118</v>
@@ -3155,7 +3155,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C23" t="s">
         <v>118</v>
@@ -3163,7 +3163,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C24" t="s">
         <v>118</v>
@@ -3171,7 +3171,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C25" t="s">
         <v>118</v>
@@ -3179,7 +3179,7 @@
     </row>
     <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -3187,7 +3187,7 @@
     </row>
     <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C28" t="s">
         <v>118</v>
@@ -3203,7 +3203,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C29" t="s">
         <v>118</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C31" t="s">
         <v>118</v>
@@ -3227,18 +3227,18 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>156</v>
@@ -3265,7 +3265,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>112</v>
@@ -3273,65 +3273,65 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="3" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="3" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C50" t="s">
         <v>118</v>
@@ -3339,12 +3339,12 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C52" t="s">
         <v>118</v>
@@ -3352,17 +3352,17 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C55" t="s">
         <v>118</v>
@@ -3370,12 +3370,12 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C57" s="43" t="s">
         <v>118</v>
@@ -3383,202 +3383,202 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>1</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>3</v>
@@ -3599,192 +3599,192 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B112" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="115" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B115" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="5" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C138" s="43" t="s">
         <v>118</v>
@@ -3792,42 +3792,42 @@
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>44</v>
@@ -3835,7 +3835,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>45</v>
@@ -3937,17 +3937,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="42" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="42" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3960,28 +3960,28 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4043,17 +4043,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="44" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4066,28 +4066,28 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>
@@ -4121,7 +4121,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -4137,7 +4137,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C3" s="8"/>
     </row>
@@ -4271,7 +4271,7 @@
     </row>
     <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C30" s="8"/>
     </row>
@@ -4340,60 +4340,60 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="9" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B49" s="45" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="45" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="45" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="45" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="45" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="45" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4433,7 +4433,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>44</v>
@@ -4466,7 +4466,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="45" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B69" s="45" t="s">
         <v>3</v>
@@ -4501,10 +4501,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C75" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -4527,15 +4527,15 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>112</v>
@@ -4561,109 +4561,109 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C87" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C93" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B95" s="5" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B96" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="45" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="B106" s="45" t="s">
         <v>1</v>
@@ -4672,27 +4672,27 @@
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
       <c r="B107" s="45" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="45" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="45" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="45" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B111" s="9" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -4700,15 +4700,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="45" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="B113" s="45" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B114" s="45" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -4774,7 +4774,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -4806,17 +4806,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="45" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4829,19 +4829,19 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4855,33 +4855,33 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C14" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>156</v>
@@ -4913,10 +4913,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4924,7 +4924,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>54</v>
@@ -4943,7 +4943,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
@@ -4970,8 +4970,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5016,17 +5016,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5070,7 +5070,7 @@
         <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -5142,19 +5142,19 @@
     </row>
     <row r="28" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5264,47 +5264,47 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>266</v>
+        <v>471</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>268</v>
+        <v>470</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -5522,7 +5522,7 @@
     </row>
     <row r="95" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="45" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -5633,7 +5633,7 @@
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C110" t="s">
         <v>167</v>
@@ -5641,7 +5641,7 @@
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C111" t="s">
         <v>167</v>
@@ -5652,36 +5652,36 @@
         <v>172</v>
       </c>
       <c r="C112" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
-        <v>173</v>
+        <v>472</v>
       </c>
       <c r="C113" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B114" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C114" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
-        <v>175</v>
+        <v>473</v>
       </c>
       <c r="C115" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B116" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C116" t="s">
         <v>167</v>
@@ -5689,7 +5689,7 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B117" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C117" t="s">
         <v>167</v>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B118" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C118" t="s">
         <v>167</v>
@@ -5705,7 +5705,7 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B119" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C119" t="s">
         <v>167</v>
@@ -5713,36 +5713,36 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B122" s="5" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C122" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B123" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C123" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B124" s="5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C124" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -5786,31 +5786,31 @@
     <row r="132" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="45" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="133" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="45" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="134" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="45" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="135" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="45" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
     </row>
     <row r="136" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="45" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -5826,7 +5826,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -5891,23 +5891,23 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B153" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C153" t="s">
         <v>229</v>
-      </c>
-      <c r="C153" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B154" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B155" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -5940,7 +5940,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
@@ -5953,7 +5953,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -5985,17 +5985,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6011,7 +6011,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C10" s="8"/>
     </row>
@@ -6020,7 +6020,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -6028,12 +6028,12 @@
         <v>121</v>
       </c>
       <c r="C12" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>56</v>
@@ -6042,7 +6042,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C15" t="s">
         <v>118</v>
@@ -6050,7 +6050,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C16" t="s">
         <v>118</v>
@@ -6058,7 +6058,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C17" t="s">
         <v>118</v>
@@ -6066,7 +6066,7 @@
     </row>
     <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C18" t="s">
         <v>118</v>
@@ -6074,7 +6074,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C19" t="s">
         <v>118</v>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C20" t="s">
         <v>118</v>
@@ -6090,7 +6090,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B22" s="45" t="s">
         <v>3</v>
@@ -6124,10 +6124,10 @@
     </row>
     <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C27" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -6156,10 +6156,10 @@
     </row>
     <row r="33" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C33" s="8"/>
     </row>
@@ -6213,10 +6213,10 @@
     </row>
     <row r="42" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C42" s="8"/>
     </row>
@@ -6250,7 +6250,7 @@
         <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6258,7 +6258,7 @@
         <v>83</v>
       </c>
       <c r="C48" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -6269,13 +6269,13 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C51" s="8"/>
     </row>
@@ -6287,19 +6287,19 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="45" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="45" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C55" s="8"/>
     </row>
@@ -6308,34 +6308,34 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C58" s="8"/>
     </row>
     <row r="59" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C59" s="8"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C61" s="8"/>
     </row>
@@ -6347,7 +6347,7 @@
     </row>
     <row r="64" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="B64" s="45" t="s">
         <v>51</v>
@@ -6355,105 +6355,105 @@
     </row>
     <row r="65" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="45" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="45" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="45" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B68" s="45" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="69" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B69" s="45" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="70" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="71" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B71" s="45" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="72" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="45" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="73" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="45" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="74" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="45" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="75" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B75" s="45" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="76" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="45" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="77" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C79" s="8"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C80" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="45" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="B84" s="45" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -6529,17 +6529,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6549,7 +6549,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -6558,13 +6558,13 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -6572,12 +6572,12 @@
         <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>100</v>
@@ -6585,15 +6585,15 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
@@ -6601,7 +6601,7 @@
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>3</v>
@@ -6614,77 +6614,77 @@
     </row>
     <row r="18" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B21" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="22" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>56</v>
@@ -6692,10 +6692,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C34" t="s">
         <v>118</v>
@@ -6703,7 +6703,7 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C35" t="s">
         <v>118</v>
@@ -6711,7 +6711,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C36" t="s">
         <v>118</v>
@@ -6719,7 +6719,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C37" t="s">
         <v>118</v>
@@ -6733,18 +6733,18 @@
         <v>156</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6767,7 +6767,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>112</v>
@@ -6775,25 +6775,25 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C49" t="s">
         <v>118</v>
@@ -6801,12 +6801,12 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C51" t="s">
         <v>118</v>
@@ -6814,77 +6814,77 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6902,7 +6902,7 @@
         <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6912,44 +6912,44 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C72" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B74" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C74" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>44</v>
@@ -6957,7 +6957,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>45</v>
@@ -7029,7 +7029,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -7061,17 +7061,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7081,13 +7081,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7095,12 +7095,12 @@
         <v>121</v>
       </c>
       <c r="C10" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -7108,63 +7108,63 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C18" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C21" t="s">
         <v>118</v>
@@ -7172,15 +7172,15 @@
     </row>
     <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="C23" t="s">
         <v>118</v>
@@ -7188,7 +7188,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C24" t="s">
         <v>118</v>
@@ -7196,7 +7196,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="C25" t="s">
         <v>118</v>
@@ -7204,7 +7204,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -7212,7 +7212,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
@@ -7228,7 +7228,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>3</v>
@@ -7243,167 +7243,167 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
       <c r="B33" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="3" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="3" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="3" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -7426,7 +7426,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>112</v>
@@ -7434,65 +7434,65 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C75" t="s">
         <v>118</v>
@@ -7500,12 +7500,12 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="C77" t="s">
         <v>118</v>
@@ -7513,102 +7513,102 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C97" t="s">
         <v>118</v>
@@ -7616,12 +7616,12 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>44</v>
@@ -7629,7 +7629,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>45</v>
@@ -7733,17 +7733,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7756,12 +7756,12 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="46" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -7771,34 +7771,34 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C13" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>56</v>
@@ -7809,7 +7809,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>3</v>
@@ -7828,12 +7828,12 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="45" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="45" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7843,7 +7843,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="45" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -7853,46 +7853,46 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="45" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="45" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="45" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="45" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="45" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
   </sheetData>
@@ -7959,19 +7959,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="22" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="22" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7984,25 +7984,25 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -8013,7 +8013,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>3</v>
@@ -8037,59 +8037,59 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="13"/>
       <c r="B19" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
@@ -8109,7 +8109,7 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="5" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C31" t="s">
         <v>118</v>
@@ -8126,7 +8126,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>156</v>
@@ -8164,15 +8164,15 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -8245,17 +8245,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -8268,33 +8268,33 @@
         <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Review related changes Related to Issue [WTI-860]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9326 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: f868cb8d47600599b12130dc470b87961caf52c1
Former-commit-id: c0420c710ab8a62bd0df1baab1f0fc7792eb7380
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="ClosingStructureFailureMechanismSectionResult">ClosingStructures!$A$15</definedName>
     <definedName name="ClosingStructuresCalculation">ClosingStructures!$A$57</definedName>
     <definedName name="ClosingStructuresInput">ClosingStructures!$A$63</definedName>
-    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$64</definedName>
+    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$62</definedName>
     <definedName name="DikeProfile">GrassCoverErosionInwards!$A$22</definedName>
     <definedName name="DuneErosionFailureMechanism">DuneErosion!$A$1</definedName>
     <definedName name="DuneErosionFailureMechanismSectionResult">DuneErosion!$A$13</definedName>
@@ -60,9 +60,9 @@
     <definedName name="GeneralWaveImpactAsphaltCoverWaveConditionsInput">WaveImpactAsphalt!$A$28</definedName>
     <definedName name="GrassCoverErosionInwardsCalculation">GrassCoverErosionInwards!$A$36</definedName>
     <definedName name="GrassCoverErosionInwardsFailureMechanism">GrassCoverErosionInwards!$A$1</definedName>
-    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$78</definedName>
+    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$69</definedName>
     <definedName name="GrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$42</definedName>
-    <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$57</definedName>
+    <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$56</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanism">GrassCoverErosionOutwards!$A$1</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanismSectionResult">GrassCoverErosionOutwards!$A$24</definedName>
     <definedName name="GrassCoverErosionOutwardsHydraulicBoundaryLocation">GrassCoverErosionOutwards!$A$15</definedName>
@@ -86,7 +86,7 @@
     <definedName name="MacrostabilityOutwardsFailureMechanismSectionResult">MacrostabilityOutwards!$A$11</definedName>
     <definedName name="MicrostabilityFailureMechanism">Microstability!$A$1</definedName>
     <definedName name="MicrostabilityFailureMechanismSectionResult">Microstability!$A$11</definedName>
-    <definedName name="OvertoppingRateAssessmentOutput">GrassCoverErosionInwards!$A$71</definedName>
+    <definedName name="OvertoppingRateAssessmentOutput">GrassCoverErosionInwards!#REF!</definedName>
     <definedName name="PipingCalculationScenario">Piping!$A$77</definedName>
     <definedName name="PipingFailureMechanism">Piping!$A$1</definedName>
     <definedName name="PipingFailureMechanismSectionResult">Piping!$A$153</definedName>
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="473">
   <si>
     <t>Description</t>
   </si>
@@ -938,9 +938,6 @@
     <t>WaveHeight</t>
   </si>
   <si>
-    <t>CalculateDikeHeight</t>
-  </si>
-  <si>
     <t>RingtoetsProject</t>
   </si>
   <si>
@@ -1451,9 +1448,6 @@
     <t>UpliftEffectiveStress</t>
   </si>
   <si>
-    <t>DikeHeightAssessmentOutput</t>
-  </si>
-  <si>
     <t>ClosingStructuresFailureMechanism</t>
   </si>
   <si>
@@ -1532,12 +1526,6 @@
     <t>OvertoppingRateCalculationType</t>
   </si>
   <si>
-    <t>OvertoppingRateAssessmentOutput</t>
-  </si>
-  <si>
-    <t>OvertoppingRate</t>
-  </si>
-  <si>
     <t>DikeProfileCollection</t>
   </si>
   <si>
@@ -1551,6 +1539,15 @@
   </si>
   <si>
     <t>DarcyPermeability.CoefficientOfVariation</t>
+  </si>
+  <si>
+    <t>DikeHeightOutput</t>
+  </si>
+  <si>
+    <t>OvertoppingRateOutput</t>
+  </si>
+  <si>
+    <t>HydraulicLoadsOutput</t>
   </si>
 </sst>
 </file>
@@ -2040,9 +2037,7 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2131,17 +2126,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2243,17 +2238,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="28" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2355,17 +2350,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2467,17 +2462,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2579,17 +2574,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2691,17 +2686,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2728,21 +2723,21 @@
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="12"/>
       <c r="B11" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C14" t="s">
         <v>118</v>
@@ -2751,7 +2746,7 @@
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C15" t="s">
         <v>118</v>
@@ -2760,7 +2755,7 @@
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C16" t="s">
         <v>118</v>
@@ -2769,7 +2764,7 @@
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C17" t="s">
         <v>118</v>
@@ -2778,7 +2773,7 @@
     <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C18" t="s">
         <v>118</v>
@@ -2787,7 +2782,7 @@
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C19" t="s">
         <v>118</v>
@@ -2795,7 +2790,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>156</v>
@@ -2827,16 +2822,16 @@
     </row>
     <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -2932,17 +2927,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3006,7 +3001,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -3038,17 +3033,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="40" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3058,18 +3053,18 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>9</v>
@@ -3086,34 +3081,34 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>260</v>
@@ -3136,7 +3131,7 @@
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
@@ -3144,7 +3139,7 @@
     </row>
     <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>248</v>
@@ -3155,7 +3150,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C23" t="s">
         <v>118</v>
@@ -3163,7 +3158,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C24" t="s">
         <v>118</v>
@@ -3171,7 +3166,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C25" t="s">
         <v>118</v>
@@ -3179,7 +3174,7 @@
     </row>
     <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -3187,7 +3182,7 @@
     </row>
     <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
@@ -3195,7 +3190,7 @@
     </row>
     <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C28" t="s">
         <v>118</v>
@@ -3203,7 +3198,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C29" t="s">
         <v>118</v>
@@ -3211,7 +3206,7 @@
     </row>
     <row r="30" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
@@ -3219,7 +3214,7 @@
     </row>
     <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B31" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C31" t="s">
         <v>118</v>
@@ -3227,18 +3222,18 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>156</v>
@@ -3265,7 +3260,7 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>112</v>
@@ -3273,55 +3268,55 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
@@ -3331,7 +3326,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C50" t="s">
         <v>118</v>
@@ -3339,12 +3334,12 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C52" t="s">
         <v>118</v>
@@ -3352,17 +3347,17 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C55" t="s">
         <v>118</v>
@@ -3370,12 +3365,12 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C57" s="43" t="s">
         <v>118</v>
@@ -3383,132 +3378,132 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="76" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="79" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
@@ -3518,7 +3513,7 @@
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
@@ -3538,47 +3533,47 @@
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B98" s="3" t="s">
         <v>1</v>
@@ -3586,7 +3581,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="8" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B99" s="3" t="s">
         <v>3</v>
@@ -3599,7 +3594,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -3609,47 +3604,47 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B105" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B106" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B107" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B111" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -3659,7 +3654,7 @@
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
@@ -3674,117 +3669,117 @@
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="118" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B118" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="121" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B121" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="124" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B124" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="127" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B127" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="128" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B128" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C138" s="43" t="s">
         <v>118</v>
@@ -3792,42 +3787,42 @@
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B145" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>44</v>
@@ -3835,7 +3830,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="8" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>45</v>
@@ -3937,17 +3932,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="42" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="42" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4043,17 +4038,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="44" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4121,7 +4116,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -4137,7 +4132,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="8"/>
     </row>
@@ -4271,7 +4266,7 @@
     </row>
     <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C30" s="8"/>
     </row>
@@ -4340,7 +4335,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4348,52 +4343,52 @@
         <v>268</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="B49" s="45" t="s">
         <v>428</v>
-      </c>
-      <c r="B49" s="45" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="45" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="45" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4466,7 +4461,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="45" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B69" s="45" t="s">
         <v>3</v>
@@ -4527,15 +4522,15 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B81" s="11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B82" s="11" t="s">
         <v>112</v>
@@ -4561,61 +4556,61 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B87" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C87" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B88" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B89" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B90" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B91" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B92" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B93" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="C93" t="s">
         <v>284</v>
-      </c>
-      <c r="C93" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="B95" s="5" t="s">
         <v>288</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B96" s="5" t="s">
         <v>268</v>
@@ -4623,47 +4618,47 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" s="5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B98" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="45" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B106" s="45" t="s">
         <v>1</v>
@@ -4672,27 +4667,27 @@
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
       <c r="B107" s="45" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="45" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="45" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="45" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B111" s="9" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -4700,15 +4695,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="45" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B113" s="45" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B114" s="45" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -4806,17 +4801,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4835,13 +4830,13 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -4881,7 +4876,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>156</v>
@@ -4913,10 +4908,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -4924,7 +4919,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B28" s="5" t="s">
         <v>54</v>
@@ -4943,7 +4938,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C30" t="s">
         <v>118</v>
@@ -4970,7 +4965,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
@@ -5016,17 +5011,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5142,19 +5137,19 @@
     </row>
     <row r="28" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5215,7 +5210,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>131</v>
       </c>
@@ -5284,7 +5279,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5294,7 +5289,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5522,7 +5517,7 @@
     </row>
     <row r="95" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="45" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -5652,15 +5647,15 @@
         <v>172</v>
       </c>
       <c r="C112" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C113" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -5668,15 +5663,15 @@
         <v>173</v>
       </c>
       <c r="C114" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C115" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -5726,7 +5721,7 @@
         <v>178</v>
       </c>
       <c r="C122" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
@@ -5734,7 +5729,7 @@
         <v>177</v>
       </c>
       <c r="C123" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
@@ -5742,7 +5737,7 @@
         <v>176</v>
       </c>
       <c r="C124" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
@@ -5786,31 +5781,31 @@
     <row r="132" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="45" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="133" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="45" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="134" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="135" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="136" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -5826,7 +5821,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -5938,10 +5933,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5985,17 +5980,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6285,175 +6280,129 @@
       </c>
       <c r="C52" s="8"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="3" t="s">
-        <v>269</v>
+    <row r="53" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="45" t="s">
+        <v>463</v>
       </c>
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="45" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C54" s="8"/>
     </row>
-    <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="45" t="s">
-        <v>466</v>
-      </c>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C55" s="8"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B56" s="9" t="s">
+        <v>209</v>
+      </c>
       <c r="C56" s="8"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>266</v>
-      </c>
+    <row r="57" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
-        <v>209</v>
+        <v>470</v>
       </c>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
-        <v>440</v>
+        <v>471</v>
       </c>
       <c r="C58" s="8"/>
     </row>
-    <row r="59" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="9" t="s">
-        <v>467</v>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="C59" s="8"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C60" s="8"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C61" s="8"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B62" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" s="8"/>
+    <row r="62" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="B62" s="45" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="45" t="s">
+        <v>422</v>
+      </c>
     </row>
     <row r="64" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
-        <v>440</v>
-      </c>
       <c r="B64" s="45" t="s">
-        <v>51</v>
+        <v>423</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="45" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="45" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="45" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B68" s="45" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B69" s="45" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>467</v>
-      </c>
-      <c r="B71" s="45" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B72" s="45" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="45" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B74" s="45" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C69" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C70" s="8"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C71" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>465</v>
+      </c>
       <c r="B75" s="45" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="45" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B78" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C78" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="C79" s="8"/>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C80" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="45" t="s">
-        <v>469</v>
-      </c>
-      <c r="B84" s="45" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
   </sheetData>
@@ -6468,10 +6417,10 @@
     <hyperlink ref="B45" location="BreakWater" display="BreakWater"/>
     <hyperlink ref="B37" location="GrassCoverErosionInwardsOutput" display="Output"/>
     <hyperlink ref="B12" location="GrassCoverErosionInwardsFailureMechanismSectionResult" display="SectionResults"/>
-    <hyperlink ref="B57" location="ProbabilityAssessmentOutput" display="ProbabilityAssessmentOutput"/>
+    <hyperlink ref="B56" location="ProbabilityAssessmentOutput" display="ProbabilityAssessmentOutput"/>
     <hyperlink ref="B9" location="GeneralGrassCoverErosionInwardsInput" display="GeneralInput"/>
+    <hyperlink ref="B57" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
     <hyperlink ref="B58" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
-    <hyperlink ref="B59" location="OvertoppingRateAssessmentOutput" display="OvertoppingRateAssessmentOutput"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -6529,17 +6478,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6549,7 +6498,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>9</v>
@@ -6558,7 +6507,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -6577,7 +6526,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>100</v>
@@ -6585,15 +6534,15 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>1</v>
@@ -6601,7 +6550,7 @@
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="8" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>3</v>
@@ -6614,17 +6563,17 @@
     </row>
     <row r="18" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="20" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B20" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="21" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
@@ -6644,22 +6593,22 @@
     </row>
     <row r="24" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B24" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="25" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
@@ -6669,17 +6618,17 @@
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -6692,7 +6641,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>248</v>
@@ -6711,7 +6660,7 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C36" t="s">
         <v>118</v>
@@ -6719,7 +6668,7 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C37" t="s">
         <v>118</v>
@@ -6733,18 +6682,18 @@
         <v>156</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -6775,25 +6724,25 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C49" t="s">
         <v>118</v>
@@ -6806,7 +6755,7 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C51" t="s">
         <v>118</v>
@@ -6814,22 +6763,22 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
@@ -6839,7 +6788,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
@@ -6859,32 +6808,32 @@
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -6902,7 +6851,7 @@
         <v>84</v>
       </c>
       <c r="C69" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -6926,7 +6875,7 @@
         <v>260</v>
       </c>
       <c r="C73" s="8" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -6949,7 +6898,7 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B78" s="3" t="s">
         <v>44</v>
@@ -6957,7 +6906,7 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B79" s="3" t="s">
         <v>45</v>
@@ -7029,7 +6978,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -7061,17 +7010,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7081,13 +7030,13 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -7100,7 +7049,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>9</v>
@@ -7108,29 +7057,29 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -7138,7 +7087,7 @@
         <v>260</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -7161,10 +7110,10 @@
     </row>
     <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C21" t="s">
         <v>118</v>
@@ -7172,10 +7121,10 @@
     </row>
     <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A22" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -7196,7 +7145,7 @@
     </row>
     <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C25" t="s">
         <v>118</v>
@@ -7204,7 +7153,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C26" t="s">
         <v>118</v>
@@ -7212,7 +7161,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C27" t="s">
         <v>118</v>
@@ -7228,7 +7177,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>3</v>
@@ -7243,7 +7192,7 @@
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -7255,79 +7204,79 @@
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="8"/>
       <c r="B36" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="8"/>
       <c r="B37" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="8"/>
       <c r="B38" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="8"/>
       <c r="B39" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="8"/>
       <c r="B40" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -7339,7 +7288,7 @@
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -7357,53 +7306,53 @@
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8"/>
       <c r="B52" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8"/>
       <c r="B53" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="8"/>
       <c r="B55" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -7426,7 +7375,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>112</v>
@@ -7434,65 +7383,65 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C75" t="s">
         <v>118</v>
@@ -7500,12 +7449,12 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C77" t="s">
         <v>118</v>
@@ -7513,52 +7462,52 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
@@ -7583,22 +7532,22 @@
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
@@ -7616,12 +7565,12 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B98" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>44</v>
@@ -7629,7 +7578,7 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B101" s="3" t="s">
         <v>45</v>
@@ -7733,17 +7682,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7761,7 +7710,7 @@
     </row>
     <row r="10" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="46" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -7798,7 +7747,7 @@
     <row r="17" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>56</v>
@@ -7809,7 +7758,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>3</v>
@@ -7828,12 +7777,12 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="45" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="45" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7843,7 +7792,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="45" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -7853,10 +7802,10 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="45" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -7867,32 +7816,32 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="45" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="45" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>
@@ -7959,19 +7908,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7990,19 +7939,19 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
       <c r="B10" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="B11" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -8013,7 +7962,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>3</v>
@@ -8037,7 +7986,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -8046,19 +7995,19 @@
         <v>268</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -8089,7 +8038,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>54</v>
@@ -8109,7 +8058,7 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C31" t="s">
         <v>118</v>
@@ -8126,7 +8075,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B34" s="9" t="s">
         <v>156</v>
@@ -8164,15 +8113,15 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -8245,17 +8194,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated OpslagMapping.xlsx Related to Issue [WTI-860]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9420 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: c602b490581f96186fbe7b4c7cf9160197cf17c8
Former-commit-id: 101d2c8cb6d1eed63711210726687e6a44e82810
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -40,7 +40,8 @@
     <definedName name="ClosingStructureFailureMechanismSectionResult">ClosingStructures!$A$15</definedName>
     <definedName name="ClosingStructuresCalculation">ClosingStructures!$A$57</definedName>
     <definedName name="ClosingStructuresInput">ClosingStructures!$A$63</definedName>
-    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$62</definedName>
+    <definedName name="DikeHeightAssessmentOutput">GrassCoverErosionInwards!$A$69</definedName>
+    <definedName name="DikeHeightOutput">GrassCoverErosionInwards!$A$62</definedName>
     <definedName name="DikeProfile">GrassCoverErosionInwards!$A$22</definedName>
     <definedName name="DuneErosionFailureMechanism">DuneErosion!$A$1</definedName>
     <definedName name="DuneErosionFailureMechanismSectionResult">DuneErosion!$A$13</definedName>
@@ -60,7 +61,7 @@
     <definedName name="GeneralWaveImpactAsphaltCoverWaveConditionsInput">WaveImpactAsphalt!$A$28</definedName>
     <definedName name="GrassCoverErosionInwardsCalculation">GrassCoverErosionInwards!$A$36</definedName>
     <definedName name="GrassCoverErosionInwardsFailureMechanism">GrassCoverErosionInwards!$A$1</definedName>
-    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$69</definedName>
+    <definedName name="GrassCoverErosionInwardsFailureMechanismSectionResult">GrassCoverErosionInwards!$A$76</definedName>
     <definedName name="GrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$42</definedName>
     <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$56</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanism">GrassCoverErosionOutwards!$A$1</definedName>
@@ -87,6 +88,7 @@
     <definedName name="MicrostabilityFailureMechanism">Microstability!$A$1</definedName>
     <definedName name="MicrostabilityFailureMechanismSectionResult">Microstability!$A$11</definedName>
     <definedName name="OvertoppingRateAssessmentOutput">GrassCoverErosionInwards!#REF!</definedName>
+    <definedName name="OvertoppingRateOutput">GrassCoverErosionInwards!$A$69</definedName>
     <definedName name="PipingCalculationScenario">Piping!$A$77</definedName>
     <definedName name="PipingFailureMechanism">Piping!$A$1</definedName>
     <definedName name="PipingFailureMechanismSectionResult">Piping!$A$153</definedName>
@@ -129,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1220" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="474">
   <si>
     <t>Description</t>
   </si>
@@ -1373,9 +1375,6 @@
     <t>HeightStructures ProbabilityAssessmentOutput</t>
   </si>
   <si>
-    <t>ClosingStructures ProbabilityAssessmentOutput</t>
-  </si>
-  <si>
     <t>StabilityPointStructures ProbabilityAssessmentOutput</t>
   </si>
   <si>
@@ -1547,14 +1546,20 @@
     <t>OvertoppingRateOutput</t>
   </si>
   <si>
-    <t>HydraulicLoadsOutput</t>
+    <t>OvertoppingRate</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ClosingStructuresProbabilityAssessmentOutput</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1610,6 +1615,22 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1676,7 +1697,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
@@ -1728,6 +1749,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="5" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="60% - Accent1" xfId="4" builtinId="32"/>
@@ -2126,17 +2149,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="26" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="26" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2238,17 +2261,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="28" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="28" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="28" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2350,17 +2373,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="30" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="30" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2462,17 +2485,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2574,17 +2597,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="34" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="34" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2640,8 +2663,8 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2686,17 +2709,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="36" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="36" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="36" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2733,7 +2756,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="50" t="s">
         <v>310</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -2788,8 +2811,8 @@
         <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>278</v>
       </c>
       <c r="B21" s="9" t="s">
@@ -2820,8 +2843,8 @@
         <v>157</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
         <v>280</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -2927,17 +2950,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="38" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="38" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2988,8 +3011,8 @@
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:C151"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B92" sqref="B92"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A147" sqref="A147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3033,17 +3056,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="40" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="40" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="37" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="40" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -3129,8 +3152,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>320</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -3221,7 +3244,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="7" t="s">
         <v>322</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -3259,7 +3282,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="7" t="s">
         <v>321</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -3277,7 +3300,7 @@
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="8"/>
       <c r="B41" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3370,7 +3393,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C57" s="43" t="s">
         <v>118</v>
@@ -3572,7 +3595,7 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="3" t="s">
+      <c r="A98" s="7" t="s">
         <v>325</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -3779,7 +3802,7 @@
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="5" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C138" s="43" t="s">
         <v>118</v>
@@ -3821,8 +3844,8 @@
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="3" t="s">
-        <v>415</v>
+      <c r="A147" s="7" t="s">
+        <v>414</v>
       </c>
       <c r="B147" s="3" t="s">
         <v>44</v>
@@ -3932,17 +3955,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="42" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="42" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="42" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4038,17 +4061,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="44" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="41" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="44" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4101,8 +4124,8 @@
   </sheetPr>
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4266,7 +4289,7 @@
     </row>
     <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C30" s="8"/>
     </row>
@@ -4335,7 +4358,7 @@
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4343,52 +4366,52 @@
         <v>268</v>
       </c>
       <c r="C45" s="43" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="46" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="47" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="13"/>
       <c r="B47" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="49" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="B49" s="45" t="s">
         <v>427</v>
-      </c>
-      <c r="B49" s="45" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="50" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="51" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B51" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="52" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="53" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="45" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4427,7 +4450,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
+      <c r="A63" s="49" t="s">
         <v>209</v>
       </c>
       <c r="B63" s="6" t="s">
@@ -4461,7 +4484,7 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="45" t="s">
-        <v>276</v>
+        <v>472</v>
       </c>
       <c r="B69" s="45" t="s">
         <v>3</v>
@@ -4521,7 +4544,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="50" t="s">
         <v>279</v>
       </c>
       <c r="B81" s="11" t="s">
@@ -4601,7 +4624,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+      <c r="A95" s="50" t="s">
         <v>287</v>
       </c>
       <c r="B95" s="5" t="s">
@@ -4628,37 +4651,37 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B99" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B100" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B101" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B102" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B103" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B104" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="45" t="s">
-        <v>457</v>
+      <c r="A106" s="7" t="s">
+        <v>456</v>
       </c>
       <c r="B106" s="45" t="s">
         <v>1</v>
@@ -4667,43 +4690,43 @@
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
       <c r="B107" s="45" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B108" s="45" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B109" s="45" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B110" s="45" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B111" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B112" s="43"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="45" t="s">
+      <c r="A113" s="7" t="s">
+        <v>459</v>
+      </c>
+      <c r="B113" s="45" t="s">
         <v>460</v>
-      </c>
-      <c r="B113" s="45" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B114" s="45" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -4756,8 +4779,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4801,17 +4824,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="45" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -4874,8 +4897,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>297</v>
       </c>
       <c r="B19" s="9" t="s">
@@ -4907,7 +4930,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="7" t="s">
         <v>298</v>
       </c>
       <c r="B25" s="9" t="s">
@@ -4918,7 +4941,7 @@
       <c r="A26" s="8"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="50" t="s">
         <v>312</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -4965,8 +4988,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B116" sqref="B116"/>
+    <sheetView topLeftCell="A142" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5011,17 +5034,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="14" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -5137,19 +5160,19 @@
     </row>
     <row r="28" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
+        <v>449</v>
+      </c>
+      <c r="B28" s="45" t="s">
         <v>450</v>
-      </c>
-      <c r="B28" s="45" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B30" s="45" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -5279,7 +5302,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" s="3" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5289,7 +5312,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5303,7 +5326,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="45" t="s">
+      <c r="A61" s="7" t="s">
         <v>134</v>
       </c>
       <c r="B61" s="45" t="s">
@@ -5517,7 +5540,7 @@
     </row>
     <row r="95" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -5652,7 +5675,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B113" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C113" t="s">
         <v>271</v>
@@ -5668,7 +5691,7 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B115" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C115" t="s">
         <v>271</v>
@@ -5781,31 +5804,31 @@
     <row r="132" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A132" s="1"/>
       <c r="B132" s="45" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="133" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A133" s="1"/>
       <c r="B133" s="45" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="134" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A134" s="1"/>
       <c r="B134" s="45" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="135" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A135" s="1"/>
       <c r="B135" s="45" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="136" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1"/>
       <c r="B136" s="45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
@@ -5821,7 +5844,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B139" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
@@ -5933,10 +5956,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5980,17 +6003,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="16" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6282,13 +6305,13 @@
     </row>
     <row r="53" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B53" s="45" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="45" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C54" s="8"/>
     </row>
@@ -6306,13 +6329,13 @@
     </row>
     <row r="57" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="9" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C58" s="8"/>
     </row>
@@ -6330,79 +6353,113 @@
     </row>
     <row r="62" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="B62" s="45" t="s">
-        <v>428</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B63" s="45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="65" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B65" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="66" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B66" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="67" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B67" s="45" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="68" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="B69" s="45" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="45" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="45" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="45" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="45" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="45" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
         <v>194</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B76" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C76" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B70" s="3" t="s">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C70" s="8"/>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B71" s="5" t="s">
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C78" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="3" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="3" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="3" t="s">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>465</v>
-      </c>
-      <c r="B75" s="45" t="s">
-        <v>451</v>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
+        <v>464</v>
+      </c>
+      <c r="B82" s="45" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -6419,8 +6476,8 @@
     <hyperlink ref="B12" location="GrassCoverErosionInwardsFailureMechanismSectionResult" display="SectionResults"/>
     <hyperlink ref="B56" location="ProbabilityAssessmentOutput" display="ProbabilityAssessmentOutput"/>
     <hyperlink ref="B9" location="GeneralGrassCoverErosionInwardsInput" display="GeneralInput"/>
-    <hyperlink ref="B57" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
-    <hyperlink ref="B58" location="DikeHeightAssessmentOutput" display="DikeHeightAssessmentOutput"/>
+    <hyperlink ref="B57" location="DikeHeightOutput" display="DikeHeightOutput"/>
+    <hyperlink ref="B58" location="OvertoppingRateOutput" display="OvertoppingRateOutput"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -6432,8 +6489,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6478,17 +6535,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -6540,8 +6597,8 @@
         <v>273</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>323</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -6632,7 +6689,7 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="7" t="s">
         <v>247</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -6675,7 +6732,7 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -6715,7 +6772,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="7" t="s">
         <v>250</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -6732,7 +6789,7 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -6897,7 +6954,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="A78" s="7" t="s">
         <v>413</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -6964,8 +7021,8 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:C104"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6978,7 +7035,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -7010,17 +7067,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7073,13 +7130,13 @@
     </row>
     <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>227</v>
       </c>
       <c r="C15" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -7108,8 +7165,8 @@
         <v>187</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>318</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -7168,7 +7225,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -7306,7 +7363,7 @@
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -7334,7 +7391,7 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="7" t="s">
         <v>328</v>
       </c>
       <c r="B57" s="3" t="s">
@@ -7374,7 +7431,7 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="7" t="s">
         <v>331</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -7391,7 +7448,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
@@ -7431,7 +7488,7 @@
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
@@ -7569,8 +7626,8 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>414</v>
+      <c r="A100" s="7" t="s">
+        <v>473</v>
       </c>
       <c r="B100" s="3" t="s">
         <v>44</v>
@@ -7637,7 +7694,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7682,17 +7739,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7710,7 +7767,7 @@
     </row>
     <row r="10" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="46" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -7746,8 +7803,8 @@
     </row>
     <row r="17" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>447</v>
+      <c r="A18" s="7" t="s">
+        <v>446</v>
       </c>
       <c r="B18" s="45" t="s">
         <v>56</v>
@@ -7757,8 +7814,8 @@
       <c r="A19" s="8"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="45" t="s">
-        <v>443</v>
+      <c r="A21" s="7" t="s">
+        <v>442</v>
       </c>
       <c r="B21" s="45" t="s">
         <v>3</v>
@@ -7777,12 +7834,12 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B24" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="45" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -7792,7 +7849,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B27" s="45" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="28" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
@@ -7801,8 +7858,8 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="45" t="s">
-        <v>448</v>
+      <c r="A30" s="7" t="s">
+        <v>447</v>
       </c>
       <c r="B30" s="45" t="s">
         <v>288</v>
@@ -7816,32 +7873,32 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="45" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="45" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="45" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="45" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" s="45" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -7862,7 +7919,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -7908,19 +7965,19 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="22" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -7986,7 +8043,7 @@
         <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -7995,19 +8052,19 @@
         <v>268</v>
       </c>
       <c r="C19" s="43" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="20" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
@@ -8194,17 +8251,17 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated database structure to be able to store Height Structure source path Related to Issue [WTI-1171]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9555 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: c00784fd15cd4832e1cb7174c210dc900bcacb5c
Former-commit-id: 2ea9760df4935174b572288f17399073635fac55
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -74,6 +74,7 @@
     <definedName name="GrassCoverSlipOffOutwardsFailureMechanism">GrassCoverSlipOffOutwards!$A$1</definedName>
     <definedName name="GrassCoverSlipOffOutwardsFailureMechanismSectionResult">GrassCoverSlipOffOutwards!$A$11</definedName>
     <definedName name="HeightStructure">HeightStructures!$A$15</definedName>
+    <definedName name="HeightStructureCollection">HeightStructures!$A$84</definedName>
     <definedName name="HeightStructuresCalculation">HeightStructures!$A$39</definedName>
     <definedName name="HeightStructuresFailureMechanism">HeightStructures!$A$1</definedName>
     <definedName name="HeightStructuresFailureMechanismSectionResult">HeightStructures!$A$72</definedName>
@@ -131,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="474">
   <si>
     <t>Description</t>
   </si>
@@ -1550,6 +1551,9 @@
   </si>
   <si>
     <t>ClosingStructuresProbabilityAssessmentOutput</t>
+  </si>
+  <si>
+    <t>HeightStructureCollection</t>
   </si>
 </sst>
 </file>
@@ -4112,8 +4116,8 @@
   </sheetPr>
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5946,8 +5950,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B82" sqref="A82:B82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6475,10 +6479,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6962,14 +6966,22 @@
         <v>16</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B81" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B82" s="3" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B84" s="45" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add persistent storage for the file location of "VoorlandProfiel" : - Corrected inconsistent column names in the database: XSourcePath --> XCollectionSourcepath for the surfacelines and stochastic soil models in Piping -- Corrected affected tests - Corrected inconsistent naming of the primary key column in the table of StabilityPointStructuresFailureMechanismMetaEntity -- Corrected affected tests - Added MetaEntities for the failure mechanisms WaveImpactAsphaltCover and StabilityStoneCover - Updated project file Ringtoets 17.2.rtd
Related to Issue [WTI-1112]


git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9570 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 06a39b1bcf6dbc7deb6b9574239c2748e553d905
Former-commit-id: 2524a81e6f9b299264ce453646304eed557fe475
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="9" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1229" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="475">
   <si>
     <t>Description</t>
   </si>
@@ -1554,6 +1554,9 @@
   </si>
   <si>
     <t>HeightStructureCollection</t>
+  </si>
+  <si>
+    <t>ForeshoreProfileCollection</t>
   </si>
 </sst>
 </file>
@@ -2653,10 +2656,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A36" sqref="A36:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2865,14 +2868,22 @@
         <v>186</v>
       </c>
     </row>
-    <row r="33" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="34" spans="2:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
       <c r="B34" s="3" t="s">
         <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="B36" s="45" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -3001,10 +3012,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:C151"/>
+  <dimension ref="A1:C153"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A147" sqref="A147"/>
+    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153:B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3864,6 +3875,14 @@
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B151" s="3" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="B153" s="45" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -4116,8 +4135,8 @@
   </sheetPr>
   <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4769,10 +4788,10 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4957,6 +4976,14 @@
       </c>
       <c r="C30" t="s">
         <v>118</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="B32" s="45" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -6479,10 +6506,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86:B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6981,6 +7008,14 @@
         <v>473</v>
       </c>
       <c r="B84" s="45" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="B86" s="45" t="s">
         <v>450</v>
       </c>
     </row>
@@ -7019,10 +7054,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:C104"/>
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:B106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7654,6 +7689,14 @@
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B104" s="3" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="B106" s="45" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -7920,7 +7963,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="A42" sqref="A42:B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8174,6 +8217,14 @@
       </c>
       <c r="B40" s="9" t="s">
         <v>287</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="45" t="s">
+        <v>474</v>
+      </c>
+      <c r="B42" s="45" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated database structure for the uniqueness of height structure id's (in a failure mechanism) and the source path of the height structures. Related to Issue [WTI-1177]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9630 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: f80af8ecb3d75a6690af6e417544b0a38c719477
Former-commit-id: 9b55851fd0aa8baca27c85094a13de1173673857
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="9" activeTab="19"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1241" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="475">
   <si>
     <t>Description</t>
   </si>
@@ -2659,7 +2659,7 @@
   <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36:B36"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2879,7 +2879,7 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="45" t="s">
+      <c r="A36" s="7" t="s">
         <v>474</v>
       </c>
       <c r="B36" s="45" t="s">
@@ -3015,7 +3015,7 @@
   <dimension ref="A1:C153"/>
   <sheetViews>
     <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153:B153"/>
+      <selection activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3878,7 +3878,7 @@
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="45" t="s">
+      <c r="A153" s="7" t="s">
         <v>474</v>
       </c>
       <c r="B153" s="45" t="s">
@@ -4790,8 +4790,8 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4979,7 +4979,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="45" t="s">
+      <c r="A32" s="7" t="s">
         <v>474</v>
       </c>
       <c r="B32" s="45" t="s">
@@ -6508,8 +6508,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86:B86"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7012,7 +7012,7 @@
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="45" t="s">
+      <c r="A86" s="7" t="s">
         <v>474</v>
       </c>
       <c r="B86" s="45" t="s">
@@ -7054,10 +7054,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A1:C106"/>
+  <dimension ref="A1:C108"/>
   <sheetViews>
     <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:B106"/>
+      <selection activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7691,11 +7691,20 @@
         <v>47</v>
       </c>
     </row>
+    <row r="105" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="45" t="s">
+      <c r="A106" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="B106" s="45" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="7" t="s">
         <v>474</v>
       </c>
-      <c r="B106" s="45" t="s">
+      <c r="B108" s="45" t="s">
         <v>450</v>
       </c>
     </row>
@@ -7963,7 +7972,7 @@
   <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:B42"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8220,7 +8229,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="45" t="s">
+      <c r="A42" s="7" t="s">
         <v>474</v>
       </c>
       <c r="B42" s="45" t="s">

</xml_diff>

<commit_message>
Add location of last selected stability point structures file: - Updated Database: -- Added uniqueness constraint to prevent non-unique items in the StabilityPointStructureCollection -- Added StabilityPointStructureCollectionSourcePath to store the sourcepath -- Updated documentation Related to Issue [WTI-1183]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@9939 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 5a3fea67496e2a50cd99e70b6df25e2fb11858ed
Former-commit-id: e270e8b7a5a567f6e9468e793539a092d2208cd3
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="4" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1245" uniqueCount="476">
   <si>
     <t>Description</t>
   </si>
@@ -1557,6 +1557,9 @@
   </si>
   <si>
     <t>ForeshoreProfileCollection</t>
+  </si>
+  <si>
+    <t>StabilityPointStructureCollection</t>
   </si>
 </sst>
 </file>
@@ -3012,10 +3015,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:C153"/>
+  <dimension ref="A1:C155"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B129" sqref="B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3882,6 +3885,14 @@
         <v>474</v>
       </c>
       <c r="B153" s="45" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" s="7" t="s">
+        <v>475</v>
+      </c>
+      <c r="B155" s="45" t="s">
         <v>450</v>
       </c>
     </row>
@@ -6508,8 +6519,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="A86" sqref="A86"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A84" sqref="A84:B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated DatabaseDesign: - Updated Excel sheet Related to Issue [WTI-1305]
git-svn-id: https://repos.deltares.nl/repos/WettelijkToetsInstrumentarium/trunk@10485 5a3db67b-de53-47b5-99c8-a1c30a6650e2

Former-commit-id: 230c344d62d144a600050675b9c14f5202c68fcd
Former-commit-id: bb77db6cecd57776067a06e85b5e41a086692e22
</commit_message>
<xml_diff>
--- a/design/OpslagMapping.xlsx
+++ b/design/OpslagMapping.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="21075" windowHeight="12735" tabRatio="1000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="21" r:id="rId1"/>
@@ -31,10 +31,10 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Piping!$B$155:$D$155</definedName>
     <definedName name="AssessmentSection">General!$A$5</definedName>
-    <definedName name="BackgroundData">General!$A$106</definedName>
-    <definedName name="BackgroundDataMeta">General!$A$113</definedName>
-    <definedName name="BreakWater">General!$A$78</definedName>
-    <definedName name="CalculationGroup">General!$A$59</definedName>
+    <definedName name="BackgroundData">General!$A$135</definedName>
+    <definedName name="BackgroundDataMeta">General!$A$142</definedName>
+    <definedName name="BreakWater">General!$A$107</definedName>
+    <definedName name="CalculationGroup">General!$A$88</definedName>
     <definedName name="ClosingStructure">ClosingStructures!$A$29</definedName>
     <definedName name="ClosingStructureFailureMechanism">ClosingStructures!$A$1</definedName>
     <definedName name="ClosingStructureFailureMechanismSectionResult">ClosingStructures!$A$15</definedName>
@@ -48,12 +48,12 @@
     <definedName name="DuneLocation">DuneErosion!$A$21</definedName>
     <definedName name="DuneLocationOutput">DuneErosion!$A$30</definedName>
     <definedName name="FailureMechanismContribution">General!$A$34</definedName>
-    <definedName name="FailureMechanismSection">General!$A$56</definedName>
-    <definedName name="ForeshoreProfile">General!$A$69</definedName>
+    <definedName name="FailureMechanismSection">General!$A$85</definedName>
+    <definedName name="ForeshoreProfile">General!$A$98</definedName>
     <definedName name="GeneralClosingStructuresInput">ClosingStructures!$A$21</definedName>
     <definedName name="GeneralDuneErosionInput">DuneErosion!$A$18</definedName>
     <definedName name="GeneralGrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$14</definedName>
-    <definedName name="GeneralGrassCoverErosionOutwardsInput">GrassCoverErosionOutwards!$A$29</definedName>
+    <definedName name="GeneralGrassCoverErosionOutwardsInput">GrassCoverErosionOutwards!$A$31</definedName>
     <definedName name="GeneralHeightStructuresInput">HeightStructures!$A$33</definedName>
     <definedName name="GeneralPipingInput">Piping!$A$60</definedName>
     <definedName name="GeneralStabilityCoverWaveConditionsInput">StabilityStoneCover!$A$14</definedName>
@@ -65,10 +65,10 @@
     <definedName name="GrassCoverErosionInwardsInput">GrassCoverErosionInwards!$A$42</definedName>
     <definedName name="GrassCoverErosionInwardsOutput">GrassCoverErosionInwards!$A$56</definedName>
     <definedName name="GrassCoverErosionOutwardsFailureMechanism">GrassCoverErosionOutwards!$A$1</definedName>
-    <definedName name="GrassCoverErosionOutwardsFailureMechanismSectionResult">GrassCoverErosionOutwards!$A$24</definedName>
+    <definedName name="GrassCoverErosionOutwardsFailureMechanismSectionResult">GrassCoverErosionOutwards!$A$26</definedName>
     <definedName name="GrassCoverErosionOutwardsHydraulicBoundaryLocation">GrassCoverErosionOutwards!$A$15</definedName>
-    <definedName name="GrassCoverErosionOutwardsWaveConditionsCalculation">GrassCoverErosionOutwards!$A$34</definedName>
-    <definedName name="GrassCoverErosionOutwardsWaveConditionsOutput">GrassCoverErosionOutwards!$A$40</definedName>
+    <definedName name="GrassCoverErosionOutwardsWaveConditionsCalculation">GrassCoverErosionOutwards!$A$36</definedName>
+    <definedName name="GrassCoverErosionOutwardsWaveConditionsOutput">GrassCoverErosionOutwards!$A$42</definedName>
     <definedName name="GrassCoverSlipOffInwardsFailureMechanism">GrassCoverSlipOffInwards!$A$1</definedName>
     <definedName name="GrassCoverSlipOffInwardsFailureMechanismSectionResult">GrassCoverSlipOffInwards!$A$11</definedName>
     <definedName name="GrassCoverSlipOffOutwardsFailureMechanism">GrassCoverSlipOffOutwards!$A$1</definedName>
@@ -81,7 +81,13 @@
     <definedName name="HeightStructuresInput">HeightStructures!$A$45</definedName>
     <definedName name="HydraulicBoundaryDatabase">General!$A$37</definedName>
     <definedName name="HydraulicBoundaryLocation">General!$A$41</definedName>
-    <definedName name="HydraulicBoundaryLocationOutput">General!$A$49</definedName>
+    <definedName name="HydraulicBoundaryLocationOutput">General!$A$51</definedName>
+    <definedName name="HydraulicLocationGeneralResult">General!$A$59</definedName>
+    <definedName name="HydraulicLocationIllustrationPoint">General!$A$73</definedName>
+    <definedName name="HydraulicLocationIllustrationPointResults">General!$A$77</definedName>
+    <definedName name="HydraulicLocationStochast">General!$A$64</definedName>
+    <definedName name="HydraulicLocationWindDirectionClosingSituationIllustrationPoint">General!$A$68</definedName>
+    <definedName name="HydraulicRealizedStochast">General!$A$80</definedName>
     <definedName name="MacrostabilityInwardsFailureMechanism">MacrostabilityInwards!$A$1</definedName>
     <definedName name="MacrostabilityInwardsFailureMechanismSectionResult">MacrostabilityInwards!$A$11</definedName>
     <definedName name="MacrostabilityOutwardsFailureMechanism">MacrostabilityOutwards!$A$1</definedName>
@@ -101,7 +107,7 @@
     <definedName name="PipingSoilProfile">Piping!$A$42</definedName>
     <definedName name="PipingStructureFailureMechanism">PipingStructure!$A$1</definedName>
     <definedName name="PipingStructureFailureMechanismSectionResult">PipingStructure!$A$11</definedName>
-    <definedName name="ProbabilityAssessmentOutput">General!$A$63</definedName>
+    <definedName name="ProbabilityAssessmentOutput">General!$A$92</definedName>
     <definedName name="ReferenceLine">General!$A$32</definedName>
     <definedName name="RingtoetsPipingSurfaceLine">Piping!$A$16</definedName>
     <definedName name="RoughnessPoint">GrassCoverErosionInwards!$A$33</definedName>
@@ -121,8 +127,8 @@
     <definedName name="TechnicalInnovationFailureMechanismSectionResult">TechnicalInnovation!$A$11</definedName>
     <definedName name="WaterPressureAsphaltCoverFailureMechanism">WaterPressureAsphaltCover!$A$1</definedName>
     <definedName name="WaterPressureAsphaltCoverFailureMechanismSectionResult">WaterPressureAsphaltCover!$A$11</definedName>
-    <definedName name="WaveConditionsInput">General!$A$81</definedName>
-    <definedName name="WaveConditionsOutput">General!$A$95</definedName>
+    <definedName name="WaveConditionsInput">General!$A$110</definedName>
+    <definedName name="WaveConditionsOutput">General!$A$124</definedName>
     <definedName name="WaveImpactAsphaltCoverFailureMechanism">WaveImpactAsphalt!$A$1</definedName>
     <definedName name="WaveImpactAsphaltCoverFailureMechanismSectionResult">WaveImpactAsphalt!$A$14</definedName>
     <definedName name="WaveImpactAsphaltCoverWaveConditionsOutput">WaveImpactAsphalt!$A$25</definedName>
@@ -132,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1244" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="494">
   <si>
     <t>Description</t>
   </si>
@@ -1557,6 +1563,63 @@
   </si>
   <si>
     <t>StabilityPointStructureCollection</t>
+  </si>
+  <si>
+    <t>Stochast</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>GeneralResult</t>
+  </si>
+  <si>
+    <t>WindDirectionClosingSituationIllustrationPoint</t>
+  </si>
+  <si>
+    <t>ClosingSituation</t>
+  </si>
+  <si>
+    <t>IllustrationPoint</t>
+  </si>
+  <si>
+    <t>Beta</t>
+  </si>
+  <si>
+    <t>RealizedStochasts</t>
+  </si>
+  <si>
+    <t>IllustrationPointResults</t>
+  </si>
+  <si>
+    <t>RealizedStochast</t>
+  </si>
+  <si>
+    <t>Realization</t>
+  </si>
+  <si>
+    <t>GoverningWindDirection.Name</t>
+  </si>
+  <si>
+    <t>GoverningWindDirection.Angle</t>
+  </si>
+  <si>
+    <t>WindDirection.Name</t>
+  </si>
+  <si>
+    <t>WindDirection.Angle</t>
+  </si>
+  <si>
+    <t>ShouldWaveHeightIllustrationPointsBeCalculated</t>
+  </si>
+  <si>
+    <t>ShouldWaterLevelIllustrationPointsBeCalculated</t>
+  </si>
+  <si>
+    <t>WTI-1305</t>
   </si>
 </sst>
 </file>
@@ -2055,7 +2118,9 @@
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2788,7 +2853,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5" t="s">
         <v>304</v>
@@ -2797,7 +2862,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5" t="s">
         <v>303</v>
@@ -2814,23 +2879,23 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
         <v>157</v>
       </c>
@@ -2846,13 +2911,13 @@
         <v>284</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="9" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>219</v>
       </c>
@@ -2863,17 +2928,17 @@
         <v>238</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>186</v>
       </c>
@@ -4141,16 +4206,16 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C115"/>
+  <dimension ref="A1:C144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
     <col min="5" max="5" width="33" customWidth="1"/>
@@ -4281,12 +4346,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="9" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
         <v>102</v>
       </c>
@@ -4367,389 +4432,552 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="3" t="s">
+    <row r="43" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="45" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="5" t="s">
+    <row r="44" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C45" s="43" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="5" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C45" s="43" t="s">
+      <c r="C47" s="43" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13"/>
-      <c r="B46" s="9" t="s">
+    <row r="48" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="9" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="9" t="s">
+    <row r="49" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="9" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+    <row r="51" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
         <v>425</v>
       </c>
-      <c r="B49" s="45" t="s">
+      <c r="B51" s="45" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="45" t="s">
+    <row r="52" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="45" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="51" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="45" t="s">
+    <row r="53" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="45" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="45" t="s">
+    <row r="54" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="45" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="45" t="s">
+    <row r="55" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="45" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="45" t="s">
+    <row r="56" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="45" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+    <row r="57" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="s">
+        <v>478</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="B60" s="6" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="s">
+        <v>475</v>
+      </c>
+      <c r="B64" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="B65" s="6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>479</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>481</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="B74" s="6" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="6" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>484</v>
+      </c>
+      <c r="B77" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:2" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="s">
+        <v>485</v>
+      </c>
+      <c r="B80" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="43" t="s">
+        <v>493</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="6" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B85" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="3" t="s">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B86" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B88" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="3" t="s">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B89" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" s="3" t="s">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B90" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C90" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B63" s="45" t="s">
+      <c r="B92" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="C63" s="8"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B64" s="45" t="s">
+      <c r="C92" s="8"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B93" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C64" s="8"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B65" s="45" t="s">
+      <c r="C93" s="8"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B94" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="8"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B66" s="45" t="s">
+      <c r="C94" s="8"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B95" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C66" s="8"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B67" s="45" t="s">
+      <c r="C95" s="8"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B96" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="C67" s="8"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
+      <c r="C96" s="8"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="B69" s="45" t="s">
+      <c r="B98" s="45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="47"/>
-      <c r="B70" s="45" t="s">
+    <row r="99" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="47"/>
+      <c r="B99" s="45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
-      <c r="B71" s="45" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="8"/>
+      <c r="B100" s="45" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="45" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="45" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="45" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="9" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="9" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="5" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B104" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C104" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="45" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B105" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B78" s="3" t="s">
+      <c r="B107" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="3" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B108" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="49" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="49" t="s">
         <v>278</v>
       </c>
-      <c r="B81" s="11" t="s">
+      <c r="B110" s="11" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>308</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B111" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="5" t="s">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B112" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="11" t="s">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B113" s="11" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="5" t="s">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B114" s="5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="5" t="s">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B115" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C115" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="5" t="s">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B116" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C116" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="5" t="s">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B117" s="5" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="5" t="s">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B118" s="5" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="5" t="s">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B119" s="5" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="5" t="s">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B120" s="5" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="5" t="s">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B121" s="5" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="5" t="s">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B122" s="5" t="s">
         <v>282</v>
       </c>
-      <c r="C93" t="s">
+      <c r="C122" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="49" t="s">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B124" s="5" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>308</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B125" s="5" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="5" t="s">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B126" s="5" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="5" t="s">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B127" s="5" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="5" t="s">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B128" s="5" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="5" t="s">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B129" s="5" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="5" t="s">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B130" s="5" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="5" t="s">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B131" s="5" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="5" t="s">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B132" s="5" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="5" t="s">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B133" s="5" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="7" t="s">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
         <v>455</v>
       </c>
-      <c r="B106" s="45" t="s">
+      <c r="B135" s="45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="8"/>
-      <c r="B107" s="45" t="s">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
+      <c r="B136" s="45" t="s">
         <v>450</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="45" t="s">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B137" s="45" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B109" s="45" t="s">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B138" s="45" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B110" s="45" t="s">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B139" s="45" t="s">
         <v>452</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B111" s="9" t="s">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B140" s="9" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B112" s="43"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="7" t="s">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B141" s="43"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="B113" s="45" t="s">
+      <c r="B142" s="45" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="45" t="s">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B143" s="45" t="s">
         <v>460</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="43"/>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B144" s="43"/>
     </row>
   </sheetData>
   <sortState ref="B82:C85">
@@ -4779,14 +5007,20 @@
     <hyperlink ref="B18" location="WaveImpactAsphaltCoverFailureMechanism" display="WaveImpactAsphaltCover"/>
     <hyperlink ref="B23" location="HeightStructuresFailureMechanism" display="HeightStructures"/>
     <hyperlink ref="B3" location="AssessmentSection" display="AssessmentSections"/>
-    <hyperlink ref="B74" location="BreakWater" display="BreakWater"/>
-    <hyperlink ref="B81" location="ForeshoreProfile" display="ForeshoreProfile"/>
-    <hyperlink ref="B82" location="HydraulicBoundaryLocation" display="HydraulicBoundaryLocation"/>
-    <hyperlink ref="B84" location="BreakWater" display="BreakWater"/>
-    <hyperlink ref="B46" location="HydraulicBoundaryLocationOutput" display="DesignWaterLevelOutput"/>
-    <hyperlink ref="B47" location="HydraulicBoundaryLocationOutput" display="WaveHeightOutput"/>
-    <hyperlink ref="B111" location="BackgroundDataMeta" display="Parameters"/>
+    <hyperlink ref="B103" location="BreakWater" display="BreakWater"/>
+    <hyperlink ref="B110" location="ForeshoreProfile" display="ForeshoreProfile"/>
+    <hyperlink ref="B111" location="HydraulicBoundaryLocation" display="HydraulicBoundaryLocation"/>
+    <hyperlink ref="B113" location="BreakWater" display="BreakWater"/>
+    <hyperlink ref="B48" location="HydraulicBoundaryLocationOutput" display="DesignWaterLevelOutput"/>
+    <hyperlink ref="B49" location="HydraulicBoundaryLocationOutput" display="WaveHeightOutput"/>
+    <hyperlink ref="B140" location="BackgroundDataMeta" display="Parameters"/>
     <hyperlink ref="B30" location="BackgroundData" display="BackgroundData"/>
+    <hyperlink ref="B57" location="HydraulicLocationGeneralResult" display="GeneralResult"/>
+    <hyperlink ref="B61" location="HydraulicLocationWindDirectionClosingSituationIllustrationPoint" display="WindDirectionClosingSituationIllustrationPoint"/>
+    <hyperlink ref="B62" location="HydraulicLocationStochast" display="Stochast"/>
+    <hyperlink ref="B71" location="HydraulicLocationIllustrationPoint" display="IllustrationPoint"/>
+    <hyperlink ref="B75" location="HydraulicLocationIllustrationPointResults" display="IllustrationPointResults"/>
+    <hyperlink ref="B74" location="HydraulicRealizedStochast" display="RealizedStochasts"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="69" fitToHeight="0" orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -4901,17 +5135,17 @@
         <v>242</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>186</v>
       </c>
@@ -4924,23 +5158,23 @@
         <v>155</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
         <v>157</v>
       </c>
@@ -5015,7 +5249,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
@@ -5203,7 +5437,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:3" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>126</v>
       </c>
@@ -5224,7 +5458,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
         <v>14</v>
       </c>
@@ -5237,7 +5471,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>128</v>
       </c>
@@ -5245,12 +5479,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>17</v>
       </c>
@@ -6511,7 +6745,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C86"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
+    <sheetView topLeftCell="A38" workbookViewId="0">
       <selection activeCell="A84" sqref="A84:B84"/>
     </sheetView>
   </sheetViews>
@@ -7972,10 +8206,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8092,155 +8326,173 @@
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13"/>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C18" s="43" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C19" s="43" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
-      <c r="B19" s="5" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="5" t="s">
         <v>267</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C21" s="43" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
-      <c r="B20" s="9" t="s">
+    <row r="22" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="9" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="9" t="s">
+    <row r="23" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="9" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A24" s="7" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B26" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" t="s">
         <v>231</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B31" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
+      <c r="C31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="C30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
-      <c r="B31" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="C31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="3" t="s">
-        <v>55</v>
+      <c r="C32" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="8"/>
+      <c r="B33" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="C33" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="B34" s="9" t="s">
-        <v>155</v>
+      <c r="A34" s="8"/>
+      <c r="B34" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
-      <c r="B35" s="9" t="s">
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="8"/>
+      <c r="B37" s="9" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36"/>
-      <c r="B36" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37"/>
-      <c r="B37" s="3" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38"/>
-      <c r="B38" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C38" t="s">
-        <v>156</v>
+      <c r="B38" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39"/>
+      <c r="B39" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="B40" s="9" t="s">
-        <v>286</v>
-      </c>
+      <c r="A40"/>
+      <c r="B40" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>473</v>
       </c>
-      <c r="B42" s="45" t="s">
+      <c r="B44" s="45" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>313</v>
       </c>
     </row>
@@ -8250,13 +8502,13 @@
     <hyperlink ref="B9" location="GrassCoverErosionOutwardsFailureMechanismSectionResult" display="SectionResults"/>
     <hyperlink ref="B11" location="GrassCoverErosionOutwardsHydraulicBoundaryLocation" display="GrassCoverErosionOutwardsHydraulicBoundaryLocations"/>
     <hyperlink ref="B10" location="CalculationGroup" display="HydraulicBoundariesCalculationGroup"/>
-    <hyperlink ref="B35" location="GrassCoverErosionOutwardsWaveConditionsOutput" display="Output"/>
-    <hyperlink ref="B34" location="WaveConditionsInput" display="InputParameters"/>
-    <hyperlink ref="B40" location="WaveConditionsOutput" display="Items"/>
+    <hyperlink ref="B37" location="GrassCoverErosionOutwardsWaveConditionsOutput" display="Output"/>
+    <hyperlink ref="B36" location="WaveConditionsInput" display="InputParameters"/>
+    <hyperlink ref="B42" location="WaveConditionsOutput" display="Items"/>
     <hyperlink ref="B13" location="GeneralGrassCoverErosionOutwardsInput" display="GeneralInput"/>
     <hyperlink ref="B12" location="ForeshoreProfile" display="ForeshoreProfiles"/>
-    <hyperlink ref="B20" location="HydraulicBoundaryLocationOutput" display="DesignWaterLevelOutput"/>
-    <hyperlink ref="B21" location="HydraulicBoundaryLocationOutput" display="WaveHeightOutput"/>
+    <hyperlink ref="B22" location="HydraulicBoundaryLocationOutput" display="DesignWaterLevelOutput"/>
+    <hyperlink ref="B23" location="HydraulicBoundaryLocationOutput" display="WaveHeightOutput"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>